<commit_message>
added working hexa driver
</commit_message>
<xml_diff>
--- a/emulator/compatibility_list.xlsx
+++ b/emulator/compatibility_list.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Φύλλο2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="OUT___Αντιγραφή" localSheetId="2">Φύλλο2!$A$1:$P$2863</definedName>
+    <definedName name="OUT___Αντιγραφή" localSheetId="2">Φύλλο2!$A$1:$P$2862</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20299,10 +20299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R141"/>
+  <dimension ref="A1:R142"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23111,6 +23111,23 @@
       </c>
       <c r="P141" t="s">
         <v>5150</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>5488</v>
+      </c>
+      <c r="B142" t="s">
+        <v>5489</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+      <c r="K142" t="s">
+        <v>60</v>
+      </c>
+      <c r="P142" t="s">
+        <v>5490</v>
       </c>
     </row>
   </sheetData>
@@ -23228,10 +23245,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2863"/>
+  <dimension ref="A1:P2862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2537" workbookViewId="0">
-      <selection activeCell="A2552" sqref="A2552:XFD2553"/>
+    <sheetView tabSelected="1" topLeftCell="A2686" workbookViewId="0">
+      <selection activeCell="A2701" sqref="A2701:XFD2701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -81342,24 +81359,21 @@
     </row>
     <row r="2701" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2701" s="1" t="s">
-        <v>5488</v>
+        <v>5491</v>
       </c>
       <c r="B2701" t="s">
-        <v>5489</v>
+        <v>5492</v>
       </c>
       <c r="C2701" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2701" t="s">
-        <v>60</v>
+        <v>605</v>
       </c>
       <c r="P2701" t="s">
-        <v>5490</v>
+        <v>5493</v>
       </c>
     </row>
     <row r="2702" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2702" s="1" t="s">
-        <v>5491</v>
+        <v>5494</v>
       </c>
       <c r="B2702" t="s">
         <v>5492</v>
@@ -81368,69 +81382,84 @@
         <v>605</v>
       </c>
       <c r="P2702" t="s">
-        <v>5493</v>
+        <v>5495</v>
       </c>
     </row>
     <row r="2703" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2703" s="1" t="s">
-        <v>5494</v>
+        <v>5496</v>
       </c>
       <c r="B2703" t="s">
-        <v>5492</v>
-      </c>
-      <c r="C2703" t="s">
-        <v>605</v>
+        <v>5497</v>
+      </c>
+      <c r="C2703">
+        <v>8080</v>
       </c>
       <c r="P2703" t="s">
-        <v>5495</v>
+        <v>5498</v>
       </c>
     </row>
     <row r="2704" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2704" s="1" t="s">
-        <v>5496</v>
+        <v>5499</v>
       </c>
       <c r="B2704" t="s">
-        <v>5497</v>
-      </c>
-      <c r="C2704">
-        <v>8080</v>
+        <v>5500</v>
+      </c>
+      <c r="C2704" t="s">
+        <v>4290</v>
+      </c>
+      <c r="D2704" t="s">
+        <v>4290</v>
+      </c>
+      <c r="E2704" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F2704" t="s">
+        <v>1422</v>
+      </c>
+      <c r="K2704" t="s">
+        <v>354</v>
+      </c>
+      <c r="L2704" t="s">
+        <v>693</v>
       </c>
       <c r="P2704" t="s">
-        <v>5498</v>
+        <v>5501</v>
       </c>
     </row>
     <row r="2705" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2705" s="1" t="s">
-        <v>5499</v>
+        <v>5502</v>
       </c>
       <c r="B2705" t="s">
-        <v>5500</v>
+        <v>5503</v>
       </c>
       <c r="C2705" t="s">
-        <v>4290</v>
+        <v>2</v>
       </c>
       <c r="D2705" t="s">
-        <v>4290</v>
+        <v>2</v>
       </c>
       <c r="E2705" t="s">
-        <v>1422</v>
+        <v>2</v>
       </c>
       <c r="F2705" t="s">
-        <v>1422</v>
+        <v>168</v>
       </c>
       <c r="K2705" t="s">
-        <v>354</v>
+        <v>60</v>
       </c>
       <c r="L2705" t="s">
-        <v>693</v>
+        <v>178</v>
       </c>
       <c r="P2705" t="s">
-        <v>5501</v>
+        <v>5504</v>
       </c>
     </row>
     <row r="2706" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2706" s="1" t="s">
-        <v>5502</v>
+        <v>5505</v>
       </c>
       <c r="B2706" t="s">
         <v>5503</v>
@@ -81454,12 +81483,12 @@
         <v>178</v>
       </c>
       <c r="P2706" t="s">
-        <v>5504</v>
+        <v>5506</v>
       </c>
     </row>
     <row r="2707" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2707" s="1" t="s">
-        <v>5505</v>
+        <v>5507</v>
       </c>
       <c r="B2707" t="s">
         <v>5503</v>
@@ -81483,12 +81512,12 @@
         <v>178</v>
       </c>
       <c r="P2707" t="s">
-        <v>5506</v>
+        <v>5508</v>
       </c>
     </row>
     <row r="2708" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2708" s="1" t="s">
-        <v>5507</v>
+        <v>5509</v>
       </c>
       <c r="B2708" t="s">
         <v>5503</v>
@@ -81512,146 +81541,134 @@
         <v>178</v>
       </c>
       <c r="P2708" t="s">
-        <v>5508</v>
+        <v>5510</v>
       </c>
     </row>
     <row r="2709" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2709" s="1" t="s">
-        <v>5509</v>
+        <v>5511</v>
       </c>
       <c r="B2709" t="s">
-        <v>5503</v>
+        <v>5512</v>
       </c>
       <c r="C2709" t="s">
         <v>2</v>
       </c>
-      <c r="D2709" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2709" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2709" t="s">
-        <v>168</v>
-      </c>
-      <c r="K2709" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2709" t="s">
-        <v>178</v>
-      </c>
       <c r="P2709" t="s">
-        <v>5510</v>
+        <v>5513</v>
       </c>
     </row>
     <row r="2710" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2710" s="1" t="s">
-        <v>5511</v>
+        <v>5517</v>
       </c>
       <c r="B2710" t="s">
-        <v>5512</v>
-      </c>
-      <c r="C2710" t="s">
-        <v>2</v>
+        <v>5518</v>
+      </c>
+      <c r="C2710">
+        <v>8080</v>
+      </c>
+      <c r="K2710" t="s">
+        <v>537</v>
       </c>
       <c r="P2710" t="s">
-        <v>5513</v>
+        <v>5519</v>
       </c>
     </row>
     <row r="2711" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2711" s="1" t="s">
-        <v>5517</v>
+        <v>5520</v>
       </c>
       <c r="B2711" t="s">
-        <v>5518</v>
-      </c>
-      <c r="C2711">
-        <v>8080</v>
+        <v>5294</v>
+      </c>
+      <c r="C2711" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2711" t="s">
+        <v>168</v>
       </c>
       <c r="K2711" t="s">
-        <v>537</v>
+        <v>357</v>
       </c>
       <c r="P2711" t="s">
-        <v>5519</v>
+        <v>5521</v>
       </c>
     </row>
     <row r="2712" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2712" s="1" t="s">
-        <v>5520</v>
+        <v>5522</v>
       </c>
       <c r="B2712" t="s">
-        <v>5294</v>
-      </c>
-      <c r="C2712" t="s">
-        <v>2</v>
+        <v>5523</v>
+      </c>
+      <c r="C2712">
+        <v>68000</v>
       </c>
       <c r="D2712" t="s">
         <v>168</v>
       </c>
       <c r="K2712" t="s">
-        <v>357</v>
+        <v>1639</v>
       </c>
       <c r="P2712" t="s">
-        <v>5521</v>
+        <v>5524</v>
       </c>
     </row>
     <row r="2713" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2713" s="1" t="s">
-        <v>5522</v>
+        <v>5525</v>
       </c>
       <c r="B2713" t="s">
-        <v>5523</v>
-      </c>
-      <c r="C2713">
-        <v>68000</v>
-      </c>
-      <c r="D2713" t="s">
-        <v>168</v>
+        <v>5526</v>
+      </c>
+      <c r="C2713" t="s">
+        <v>536</v>
       </c>
       <c r="K2713" t="s">
-        <v>1639</v>
+        <v>60</v>
       </c>
       <c r="P2713" t="s">
-        <v>5524</v>
+        <v>5527</v>
       </c>
     </row>
     <row r="2714" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2714" s="1" t="s">
-        <v>5525</v>
+        <v>5528</v>
       </c>
       <c r="B2714" t="s">
-        <v>5526</v>
+        <v>5529</v>
       </c>
       <c r="C2714" t="s">
-        <v>536</v>
+        <v>2</v>
       </c>
       <c r="K2714" t="s">
-        <v>60</v>
+        <v>537</v>
       </c>
       <c r="P2714" t="s">
-        <v>5527</v>
+        <v>6564</v>
       </c>
     </row>
     <row r="2715" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2715" s="1" t="s">
-        <v>5528</v>
+        <v>5530</v>
       </c>
       <c r="B2715" t="s">
-        <v>5529</v>
+        <v>5531</v>
       </c>
       <c r="C2715" t="s">
         <v>2</v>
       </c>
       <c r="K2715" t="s">
-        <v>537</v>
+        <v>63</v>
       </c>
       <c r="P2715" t="s">
-        <v>6564</v>
+        <v>5532</v>
       </c>
     </row>
     <row r="2716" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2716" s="1" t="s">
-        <v>5530</v>
+        <v>5533</v>
       </c>
       <c r="B2716" t="s">
         <v>5531</v>
@@ -81663,80 +81680,83 @@
         <v>63</v>
       </c>
       <c r="P2716" t="s">
-        <v>5532</v>
+        <v>5534</v>
       </c>
     </row>
     <row r="2717" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2717" s="1" t="s">
-        <v>5533</v>
+        <v>5535</v>
       </c>
       <c r="B2717" t="s">
-        <v>5531</v>
+        <v>5536</v>
       </c>
       <c r="C2717" t="s">
         <v>2</v>
       </c>
       <c r="K2717" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="P2717" t="s">
-        <v>5534</v>
+        <v>5537</v>
       </c>
     </row>
     <row r="2718" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2718" s="1" t="s">
-        <v>5535</v>
+        <v>5538</v>
       </c>
       <c r="B2718" t="s">
-        <v>5536</v>
+        <v>5539</v>
       </c>
       <c r="C2718" t="s">
         <v>2</v>
       </c>
       <c r="K2718" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="P2718" t="s">
-        <v>5537</v>
+        <v>5540</v>
       </c>
     </row>
     <row r="2719" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2719" s="1" t="s">
-        <v>5538</v>
+        <v>5541</v>
       </c>
       <c r="B2719" t="s">
-        <v>5539</v>
+        <v>5542</v>
       </c>
       <c r="C2719" t="s">
         <v>2</v>
       </c>
       <c r="K2719" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="P2719" t="s">
-        <v>5540</v>
+        <v>5543</v>
       </c>
     </row>
     <row r="2720" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2720" s="1" t="s">
-        <v>5541</v>
+        <v>5544</v>
       </c>
       <c r="B2720" t="s">
-        <v>5542</v>
+        <v>5545</v>
       </c>
       <c r="C2720" t="s">
         <v>2</v>
       </c>
+      <c r="D2720" t="s">
+        <v>2</v>
+      </c>
       <c r="K2720" t="s">
-        <v>60</v>
+        <v>693</v>
       </c>
       <c r="P2720" t="s">
-        <v>5543</v>
+        <v>6565</v>
       </c>
     </row>
     <row r="2721" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2721" s="1" t="s">
-        <v>5544</v>
+        <v>5546</v>
       </c>
       <c r="B2721" t="s">
         <v>5545</v>
@@ -81751,32 +81771,29 @@
         <v>693</v>
       </c>
       <c r="P2721" t="s">
-        <v>6565</v>
+        <v>6566</v>
       </c>
     </row>
     <row r="2722" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2722" s="1" t="s">
-        <v>5546</v>
+        <v>5547</v>
       </c>
       <c r="B2722" t="s">
-        <v>5545</v>
+        <v>5548</v>
       </c>
       <c r="C2722" t="s">
         <v>2</v>
       </c>
-      <c r="D2722" t="s">
-        <v>2</v>
-      </c>
       <c r="K2722" t="s">
-        <v>693</v>
+        <v>60</v>
       </c>
       <c r="P2722" t="s">
-        <v>6566</v>
+        <v>5549</v>
       </c>
     </row>
     <row r="2723" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2723" s="1" t="s">
-        <v>5547</v>
+        <v>5550</v>
       </c>
       <c r="B2723" t="s">
         <v>5548</v>
@@ -81784,16 +81801,25 @@
       <c r="C2723" t="s">
         <v>2</v>
       </c>
+      <c r="D2723" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2723" t="s">
+        <v>168</v>
+      </c>
       <c r="K2723" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2723" t="s">
         <v>60</v>
       </c>
       <c r="P2723" t="s">
-        <v>5549</v>
+        <v>5551</v>
       </c>
     </row>
     <row r="2724" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2724" s="1" t="s">
-        <v>5550</v>
+        <v>5552</v>
       </c>
       <c r="B2724" t="s">
         <v>5548</v>
@@ -81814,55 +81840,43 @@
         <v>60</v>
       </c>
       <c r="P2724" t="s">
-        <v>5551</v>
+        <v>5553</v>
       </c>
     </row>
     <row r="2725" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2725" s="1" t="s">
-        <v>5552</v>
+        <v>5554</v>
       </c>
       <c r="B2725" t="s">
-        <v>5548</v>
-      </c>
-      <c r="C2725" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2725" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2725" t="s">
-        <v>168</v>
+        <v>5555</v>
+      </c>
+      <c r="C2725">
+        <v>68000</v>
       </c>
       <c r="K2725" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2725" t="s">
-        <v>60</v>
+        <v>2076</v>
       </c>
       <c r="P2725" t="s">
-        <v>5553</v>
+        <v>5556</v>
       </c>
     </row>
     <row r="2726" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2726" s="1" t="s">
-        <v>5554</v>
+        <v>5557</v>
       </c>
       <c r="B2726" t="s">
-        <v>5555</v>
-      </c>
-      <c r="C2726">
-        <v>68000</v>
-      </c>
-      <c r="K2726" t="s">
-        <v>2076</v>
+        <v>5558</v>
+      </c>
+      <c r="C2726" t="s">
+        <v>2</v>
       </c>
       <c r="P2726" t="s">
-        <v>5556</v>
+        <v>5559</v>
       </c>
     </row>
     <row r="2727" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2727" s="1" t="s">
-        <v>5557</v>
+        <v>5560</v>
       </c>
       <c r="B2727" t="s">
         <v>5558</v>
@@ -81871,26 +81885,32 @@
         <v>2</v>
       </c>
       <c r="P2727" t="s">
-        <v>5559</v>
+        <v>5561</v>
       </c>
     </row>
     <row r="2728" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2728" s="1" t="s">
-        <v>5560</v>
+        <v>5562</v>
       </c>
       <c r="B2728" t="s">
-        <v>5558</v>
-      </c>
-      <c r="C2728" t="s">
-        <v>2</v>
+        <v>5563</v>
+      </c>
+      <c r="C2728">
+        <v>68000</v>
+      </c>
+      <c r="D2728" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2728" t="s">
+        <v>1790</v>
       </c>
       <c r="P2728" t="s">
-        <v>5561</v>
+        <v>5564</v>
       </c>
     </row>
     <row r="2729" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2729" s="1" t="s">
-        <v>5562</v>
+        <v>5565</v>
       </c>
       <c r="B2729" t="s">
         <v>5563</v>
@@ -81905,12 +81925,12 @@
         <v>1790</v>
       </c>
       <c r="P2729" t="s">
-        <v>5564</v>
+        <v>6567</v>
       </c>
     </row>
     <row r="2730" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2730" s="1" t="s">
-        <v>5565</v>
+        <v>5566</v>
       </c>
       <c r="B2730" t="s">
         <v>5563</v>
@@ -81925,12 +81945,12 @@
         <v>1790</v>
       </c>
       <c r="P2730" t="s">
-        <v>6567</v>
+        <v>5567</v>
       </c>
     </row>
     <row r="2731" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2731" s="1" t="s">
-        <v>5566</v>
+        <v>5568</v>
       </c>
       <c r="B2731" t="s">
         <v>5563</v>
@@ -81945,12 +81965,12 @@
         <v>1790</v>
       </c>
       <c r="P2731" t="s">
-        <v>5567</v>
+        <v>5569</v>
       </c>
     </row>
     <row r="2732" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2732" s="1" t="s">
-        <v>5568</v>
+        <v>5570</v>
       </c>
       <c r="B2732" t="s">
         <v>5563</v>
@@ -81965,12 +81985,12 @@
         <v>1790</v>
       </c>
       <c r="P2732" t="s">
-        <v>5569</v>
+        <v>5571</v>
       </c>
     </row>
     <row r="2733" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2733" s="1" t="s">
-        <v>5570</v>
+        <v>5572</v>
       </c>
       <c r="B2733" t="s">
         <v>5563</v>
@@ -81985,12 +82005,12 @@
         <v>1790</v>
       </c>
       <c r="P2733" t="s">
-        <v>5571</v>
+        <v>5573</v>
       </c>
     </row>
     <row r="2734" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2734" s="1" t="s">
-        <v>5572</v>
+        <v>5574</v>
       </c>
       <c r="B2734" t="s">
         <v>5563</v>
@@ -82005,12 +82025,12 @@
         <v>1790</v>
       </c>
       <c r="P2734" t="s">
-        <v>5573</v>
+        <v>5575</v>
       </c>
     </row>
     <row r="2735" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2735" s="1" t="s">
-        <v>5574</v>
+        <v>5576</v>
       </c>
       <c r="B2735" t="s">
         <v>5563</v>
@@ -82025,12 +82045,12 @@
         <v>1790</v>
       </c>
       <c r="P2735" t="s">
-        <v>5575</v>
+        <v>5577</v>
       </c>
     </row>
     <row r="2736" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2736" s="1" t="s">
-        <v>5576</v>
+        <v>5578</v>
       </c>
       <c r="B2736" t="s">
         <v>5563</v>
@@ -82045,12 +82065,12 @@
         <v>1790</v>
       </c>
       <c r="P2736" t="s">
-        <v>5577</v>
+        <v>6568</v>
       </c>
     </row>
     <row r="2737" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2737" s="1" t="s">
-        <v>5578</v>
+        <v>5579</v>
       </c>
       <c r="B2737" t="s">
         <v>5563</v>
@@ -82065,12 +82085,12 @@
         <v>1790</v>
       </c>
       <c r="P2737" t="s">
-        <v>6568</v>
+        <v>5580</v>
       </c>
     </row>
     <row r="2738" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2738" s="1" t="s">
-        <v>5579</v>
+        <v>5581</v>
       </c>
       <c r="B2738" t="s">
         <v>5563</v>
@@ -82085,12 +82105,12 @@
         <v>1790</v>
       </c>
       <c r="P2738" t="s">
-        <v>5580</v>
+        <v>5582</v>
       </c>
     </row>
     <row r="2739" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2739" s="1" t="s">
-        <v>5581</v>
+        <v>5583</v>
       </c>
       <c r="B2739" t="s">
         <v>5563</v>
@@ -82105,12 +82125,12 @@
         <v>1790</v>
       </c>
       <c r="P2739" t="s">
-        <v>5582</v>
+        <v>5584</v>
       </c>
     </row>
     <row r="2740" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2740" s="1" t="s">
-        <v>5583</v>
+        <v>5585</v>
       </c>
       <c r="B2740" t="s">
         <v>5563</v>
@@ -82125,12 +82145,12 @@
         <v>1790</v>
       </c>
       <c r="P2740" t="s">
-        <v>5584</v>
+        <v>5586</v>
       </c>
     </row>
     <row r="2741" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2741" s="1" t="s">
-        <v>5585</v>
+        <v>5587</v>
       </c>
       <c r="B2741" t="s">
         <v>5563</v>
@@ -82145,12 +82165,12 @@
         <v>1790</v>
       </c>
       <c r="P2741" t="s">
-        <v>5586</v>
+        <v>5588</v>
       </c>
     </row>
     <row r="2742" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2742" s="1" t="s">
-        <v>5587</v>
+        <v>5589</v>
       </c>
       <c r="B2742" t="s">
         <v>5563</v>
@@ -82165,12 +82185,12 @@
         <v>1790</v>
       </c>
       <c r="P2742" t="s">
-        <v>5588</v>
+        <v>6569</v>
       </c>
     </row>
     <row r="2743" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2743" s="1" t="s">
-        <v>5589</v>
+        <v>5590</v>
       </c>
       <c r="B2743" t="s">
         <v>5563</v>
@@ -82185,12 +82205,12 @@
         <v>1790</v>
       </c>
       <c r="P2743" t="s">
-        <v>6569</v>
+        <v>6570</v>
       </c>
     </row>
     <row r="2744" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2744" s="1" t="s">
-        <v>5590</v>
+        <v>5591</v>
       </c>
       <c r="B2744" t="s">
         <v>5563</v>
@@ -82205,12 +82225,12 @@
         <v>1790</v>
       </c>
       <c r="P2744" t="s">
-        <v>6570</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="2745" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2745" s="1" t="s">
-        <v>5591</v>
+        <v>5593</v>
       </c>
       <c r="B2745" t="s">
         <v>5563</v>
@@ -82225,12 +82245,12 @@
         <v>1790</v>
       </c>
       <c r="P2745" t="s">
-        <v>5592</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="2746" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2746" s="1" t="s">
-        <v>5593</v>
+        <v>5595</v>
       </c>
       <c r="B2746" t="s">
         <v>5563</v>
@@ -82245,12 +82265,12 @@
         <v>1790</v>
       </c>
       <c r="P2746" t="s">
-        <v>5594</v>
+        <v>5596</v>
       </c>
     </row>
     <row r="2747" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2747" s="1" t="s">
-        <v>5595</v>
+        <v>5597</v>
       </c>
       <c r="B2747" t="s">
         <v>5563</v>
@@ -82265,12 +82285,12 @@
         <v>1790</v>
       </c>
       <c r="P2747" t="s">
-        <v>5596</v>
+        <v>5598</v>
       </c>
     </row>
     <row r="2748" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2748" s="1" t="s">
-        <v>5597</v>
+        <v>5599</v>
       </c>
       <c r="B2748" t="s">
         <v>5563</v>
@@ -82285,12 +82305,12 @@
         <v>1790</v>
       </c>
       <c r="P2748" t="s">
-        <v>5598</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="2749" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2749" s="1" t="s">
-        <v>5599</v>
+        <v>5601</v>
       </c>
       <c r="B2749" t="s">
         <v>5563</v>
@@ -82305,12 +82325,12 @@
         <v>1790</v>
       </c>
       <c r="P2749" t="s">
-        <v>5600</v>
+        <v>5602</v>
       </c>
     </row>
     <row r="2750" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2750" s="1" t="s">
-        <v>5601</v>
+        <v>5603</v>
       </c>
       <c r="B2750" t="s">
         <v>5563</v>
@@ -82325,12 +82345,12 @@
         <v>1790</v>
       </c>
       <c r="P2750" t="s">
-        <v>5602</v>
+        <v>6571</v>
       </c>
     </row>
     <row r="2751" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2751" s="1" t="s">
-        <v>5603</v>
+        <v>5604</v>
       </c>
       <c r="B2751" t="s">
         <v>5563</v>
@@ -82345,12 +82365,12 @@
         <v>1790</v>
       </c>
       <c r="P2751" t="s">
-        <v>6571</v>
+        <v>5605</v>
       </c>
     </row>
     <row r="2752" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2752" s="1" t="s">
-        <v>5604</v>
+        <v>5606</v>
       </c>
       <c r="B2752" t="s">
         <v>5563</v>
@@ -82365,12 +82385,12 @@
         <v>1790</v>
       </c>
       <c r="P2752" t="s">
-        <v>5605</v>
+        <v>5607</v>
       </c>
     </row>
     <row r="2753" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2753" s="1" t="s">
-        <v>5606</v>
+        <v>5608</v>
       </c>
       <c r="B2753" t="s">
         <v>5563</v>
@@ -82385,12 +82405,12 @@
         <v>1790</v>
       </c>
       <c r="P2753" t="s">
-        <v>5607</v>
+        <v>5609</v>
       </c>
     </row>
     <row r="2754" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2754" s="1" t="s">
-        <v>5608</v>
+        <v>5610</v>
       </c>
       <c r="B2754" t="s">
         <v>5563</v>
@@ -82405,12 +82425,12 @@
         <v>1790</v>
       </c>
       <c r="P2754" t="s">
-        <v>5609</v>
+        <v>6572</v>
       </c>
     </row>
     <row r="2755" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2755" s="1" t="s">
-        <v>5610</v>
+        <v>5611</v>
       </c>
       <c r="B2755" t="s">
         <v>5563</v>
@@ -82425,12 +82445,12 @@
         <v>1790</v>
       </c>
       <c r="P2755" t="s">
-        <v>6572</v>
+        <v>6573</v>
       </c>
     </row>
     <row r="2756" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2756" s="1" t="s">
-        <v>5611</v>
+        <v>5612</v>
       </c>
       <c r="B2756" t="s">
         <v>5563</v>
@@ -82445,12 +82465,12 @@
         <v>1790</v>
       </c>
       <c r="P2756" t="s">
-        <v>6573</v>
+        <v>6574</v>
       </c>
     </row>
     <row r="2757" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2757" s="1" t="s">
-        <v>5612</v>
+        <v>5613</v>
       </c>
       <c r="B2757" t="s">
         <v>5563</v>
@@ -82465,12 +82485,12 @@
         <v>1790</v>
       </c>
       <c r="P2757" t="s">
-        <v>6574</v>
+        <v>5614</v>
       </c>
     </row>
     <row r="2758" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2758" s="1" t="s">
-        <v>5613</v>
+        <v>5615</v>
       </c>
       <c r="B2758" t="s">
         <v>5563</v>
@@ -82485,12 +82505,12 @@
         <v>1790</v>
       </c>
       <c r="P2758" t="s">
-        <v>5614</v>
+        <v>5616</v>
       </c>
     </row>
     <row r="2759" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2759" s="1" t="s">
-        <v>5615</v>
+        <v>5617</v>
       </c>
       <c r="B2759" t="s">
         <v>5563</v>
@@ -82505,12 +82525,12 @@
         <v>1790</v>
       </c>
       <c r="P2759" t="s">
-        <v>5616</v>
+        <v>6575</v>
       </c>
     </row>
     <row r="2760" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2760" s="1" t="s">
-        <v>5617</v>
+        <v>5618</v>
       </c>
       <c r="B2760" t="s">
         <v>5563</v>
@@ -82525,12 +82545,12 @@
         <v>1790</v>
       </c>
       <c r="P2760" t="s">
-        <v>6575</v>
+        <v>5619</v>
       </c>
     </row>
     <row r="2761" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2761" s="1" t="s">
-        <v>5618</v>
+        <v>5620</v>
       </c>
       <c r="B2761" t="s">
         <v>5563</v>
@@ -82545,12 +82565,12 @@
         <v>1790</v>
       </c>
       <c r="P2761" t="s">
-        <v>5619</v>
+        <v>6576</v>
       </c>
     </row>
     <row r="2762" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2762" s="1" t="s">
-        <v>5620</v>
+        <v>5621</v>
       </c>
       <c r="B2762" t="s">
         <v>5563</v>
@@ -82565,12 +82585,12 @@
         <v>1790</v>
       </c>
       <c r="P2762" t="s">
-        <v>6576</v>
+        <v>5622</v>
       </c>
     </row>
     <row r="2763" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2763" s="1" t="s">
-        <v>5621</v>
+        <v>5623</v>
       </c>
       <c r="B2763" t="s">
         <v>5563</v>
@@ -82585,12 +82605,12 @@
         <v>1790</v>
       </c>
       <c r="P2763" t="s">
-        <v>5622</v>
+        <v>5624</v>
       </c>
     </row>
     <row r="2764" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2764" s="1" t="s">
-        <v>5623</v>
+        <v>5625</v>
       </c>
       <c r="B2764" t="s">
         <v>5563</v>
@@ -82605,12 +82625,12 @@
         <v>1790</v>
       </c>
       <c r="P2764" t="s">
-        <v>5624</v>
+        <v>6577</v>
       </c>
     </row>
     <row r="2765" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2765" s="1" t="s">
-        <v>5625</v>
+        <v>5626</v>
       </c>
       <c r="B2765" t="s">
         <v>5563</v>
@@ -82625,12 +82645,12 @@
         <v>1790</v>
       </c>
       <c r="P2765" t="s">
-        <v>6577</v>
+        <v>6578</v>
       </c>
     </row>
     <row r="2766" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2766" s="1" t="s">
-        <v>5626</v>
+        <v>5627</v>
       </c>
       <c r="B2766" t="s">
         <v>5563</v>
@@ -82645,12 +82665,12 @@
         <v>1790</v>
       </c>
       <c r="P2766" t="s">
-        <v>6578</v>
+        <v>5628</v>
       </c>
     </row>
     <row r="2767" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2767" s="1" t="s">
-        <v>5627</v>
+        <v>5629</v>
       </c>
       <c r="B2767" t="s">
         <v>5563</v>
@@ -82665,12 +82685,12 @@
         <v>1790</v>
       </c>
       <c r="P2767" t="s">
-        <v>5628</v>
+        <v>6579</v>
       </c>
     </row>
     <row r="2768" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2768" s="1" t="s">
-        <v>5629</v>
+        <v>5630</v>
       </c>
       <c r="B2768" t="s">
         <v>5563</v>
@@ -82685,12 +82705,12 @@
         <v>1790</v>
       </c>
       <c r="P2768" t="s">
-        <v>6579</v>
+        <v>6580</v>
       </c>
     </row>
     <row r="2769" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2769" s="1" t="s">
-        <v>5630</v>
+        <v>5631</v>
       </c>
       <c r="B2769" t="s">
         <v>5563</v>
@@ -82705,12 +82725,12 @@
         <v>1790</v>
       </c>
       <c r="P2769" t="s">
-        <v>6580</v>
+        <v>6581</v>
       </c>
     </row>
     <row r="2770" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2770" s="1" t="s">
-        <v>5631</v>
+        <v>5632</v>
       </c>
       <c r="B2770" t="s">
         <v>5563</v>
@@ -82725,12 +82745,12 @@
         <v>1790</v>
       </c>
       <c r="P2770" t="s">
-        <v>6581</v>
+        <v>6582</v>
       </c>
     </row>
     <row r="2771" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2771" s="1" t="s">
-        <v>5632</v>
+        <v>5633</v>
       </c>
       <c r="B2771" t="s">
         <v>5563</v>
@@ -82745,12 +82765,12 @@
         <v>1790</v>
       </c>
       <c r="P2771" t="s">
-        <v>6582</v>
+        <v>6583</v>
       </c>
     </row>
     <row r="2772" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2772" s="1" t="s">
-        <v>5633</v>
+        <v>5634</v>
       </c>
       <c r="B2772" t="s">
         <v>5563</v>
@@ -82765,12 +82785,12 @@
         <v>1790</v>
       </c>
       <c r="P2772" t="s">
-        <v>6583</v>
+        <v>6584</v>
       </c>
     </row>
     <row r="2773" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2773" s="1" t="s">
-        <v>5634</v>
+        <v>5635</v>
       </c>
       <c r="B2773" t="s">
         <v>5563</v>
@@ -82785,12 +82805,12 @@
         <v>1790</v>
       </c>
       <c r="P2773" t="s">
-        <v>6584</v>
+        <v>6585</v>
       </c>
     </row>
     <row r="2774" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2774" s="1" t="s">
-        <v>5635</v>
+        <v>5636</v>
       </c>
       <c r="B2774" t="s">
         <v>5563</v>
@@ -82805,12 +82825,12 @@
         <v>1790</v>
       </c>
       <c r="P2774" t="s">
-        <v>6585</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="2775" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2775" s="1" t="s">
-        <v>5636</v>
+        <v>5638</v>
       </c>
       <c r="B2775" t="s">
         <v>5563</v>
@@ -82825,12 +82845,12 @@
         <v>1790</v>
       </c>
       <c r="P2775" t="s">
-        <v>5637</v>
+        <v>5639</v>
       </c>
     </row>
     <row r="2776" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2776" s="1" t="s">
-        <v>5638</v>
+        <v>5640</v>
       </c>
       <c r="B2776" t="s">
         <v>5563</v>
@@ -82845,12 +82865,12 @@
         <v>1790</v>
       </c>
       <c r="P2776" t="s">
-        <v>5639</v>
+        <v>5641</v>
       </c>
     </row>
     <row r="2777" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2777" s="1" t="s">
-        <v>5640</v>
+        <v>5642</v>
       </c>
       <c r="B2777" t="s">
         <v>5563</v>
@@ -82865,12 +82885,12 @@
         <v>1790</v>
       </c>
       <c r="P2777" t="s">
-        <v>5641</v>
+        <v>6586</v>
       </c>
     </row>
     <row r="2778" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2778" s="1" t="s">
-        <v>5642</v>
+        <v>5643</v>
       </c>
       <c r="B2778" t="s">
         <v>5563</v>
@@ -82885,12 +82905,12 @@
         <v>1790</v>
       </c>
       <c r="P2778" t="s">
-        <v>6586</v>
+        <v>5644</v>
       </c>
     </row>
     <row r="2779" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2779" s="1" t="s">
-        <v>5643</v>
+        <v>5645</v>
       </c>
       <c r="B2779" t="s">
         <v>5563</v>
@@ -82905,12 +82925,12 @@
         <v>1790</v>
       </c>
       <c r="P2779" t="s">
-        <v>5644</v>
+        <v>5646</v>
       </c>
     </row>
     <row r="2780" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2780" s="1" t="s">
-        <v>5645</v>
+        <v>5647</v>
       </c>
       <c r="B2780" t="s">
         <v>5563</v>
@@ -82925,12 +82945,12 @@
         <v>1790</v>
       </c>
       <c r="P2780" t="s">
-        <v>5646</v>
+        <v>6587</v>
       </c>
     </row>
     <row r="2781" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2781" s="1" t="s">
-        <v>5647</v>
+        <v>5648</v>
       </c>
       <c r="B2781" t="s">
         <v>5563</v>
@@ -82945,12 +82965,12 @@
         <v>1790</v>
       </c>
       <c r="P2781" t="s">
-        <v>6587</v>
+        <v>5649</v>
       </c>
     </row>
     <row r="2782" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2782" s="1" t="s">
-        <v>5648</v>
+        <v>5650</v>
       </c>
       <c r="B2782" t="s">
         <v>5563</v>
@@ -82965,12 +82985,12 @@
         <v>1790</v>
       </c>
       <c r="P2782" t="s">
-        <v>5649</v>
+        <v>6588</v>
       </c>
     </row>
     <row r="2783" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2783" s="1" t="s">
-        <v>5650</v>
+        <v>5651</v>
       </c>
       <c r="B2783" t="s">
         <v>5563</v>
@@ -82985,12 +83005,12 @@
         <v>1790</v>
       </c>
       <c r="P2783" t="s">
-        <v>6588</v>
+        <v>6589</v>
       </c>
     </row>
     <row r="2784" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2784" s="1" t="s">
-        <v>5651</v>
+        <v>5652</v>
       </c>
       <c r="B2784" t="s">
         <v>5563</v>
@@ -83005,12 +83025,12 @@
         <v>1790</v>
       </c>
       <c r="P2784" t="s">
-        <v>6589</v>
+        <v>6590</v>
       </c>
     </row>
     <row r="2785" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2785" s="1" t="s">
-        <v>5652</v>
+        <v>5653</v>
       </c>
       <c r="B2785" t="s">
         <v>5563</v>
@@ -83025,12 +83045,12 @@
         <v>1790</v>
       </c>
       <c r="P2785" t="s">
-        <v>6590</v>
+        <v>6591</v>
       </c>
     </row>
     <row r="2786" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2786" s="1" t="s">
-        <v>5653</v>
+        <v>5654</v>
       </c>
       <c r="B2786" t="s">
         <v>5563</v>
@@ -83045,12 +83065,12 @@
         <v>1790</v>
       </c>
       <c r="P2786" t="s">
-        <v>6591</v>
+        <v>6592</v>
       </c>
     </row>
     <row r="2787" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2787" s="1" t="s">
-        <v>5654</v>
+        <v>5655</v>
       </c>
       <c r="B2787" t="s">
         <v>5563</v>
@@ -83065,12 +83085,12 @@
         <v>1790</v>
       </c>
       <c r="P2787" t="s">
-        <v>6592</v>
+        <v>6593</v>
       </c>
     </row>
     <row r="2788" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2788" s="1" t="s">
-        <v>5655</v>
+        <v>5656</v>
       </c>
       <c r="B2788" t="s">
         <v>5563</v>
@@ -83085,12 +83105,12 @@
         <v>1790</v>
       </c>
       <c r="P2788" t="s">
-        <v>6593</v>
+        <v>5657</v>
       </c>
     </row>
     <row r="2789" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2789" s="1" t="s">
-        <v>5656</v>
+        <v>5658</v>
       </c>
       <c r="B2789" t="s">
         <v>5563</v>
@@ -83105,12 +83125,12 @@
         <v>1790</v>
       </c>
       <c r="P2789" t="s">
-        <v>5657</v>
+        <v>6594</v>
       </c>
     </row>
     <row r="2790" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2790" s="1" t="s">
-        <v>5658</v>
+        <v>5659</v>
       </c>
       <c r="B2790" t="s">
         <v>5563</v>
@@ -83125,12 +83145,12 @@
         <v>1790</v>
       </c>
       <c r="P2790" t="s">
-        <v>6594</v>
+        <v>6595</v>
       </c>
     </row>
     <row r="2791" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2791" s="1" t="s">
-        <v>5659</v>
+        <v>5660</v>
       </c>
       <c r="B2791" t="s">
         <v>5563</v>
@@ -83145,12 +83165,12 @@
         <v>1790</v>
       </c>
       <c r="P2791" t="s">
-        <v>6595</v>
+        <v>5661</v>
       </c>
     </row>
     <row r="2792" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2792" s="1" t="s">
-        <v>5660</v>
+        <v>5662</v>
       </c>
       <c r="B2792" t="s">
         <v>5563</v>
@@ -83165,12 +83185,12 @@
         <v>1790</v>
       </c>
       <c r="P2792" t="s">
-        <v>5661</v>
+        <v>5663</v>
       </c>
     </row>
     <row r="2793" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2793" s="1" t="s">
-        <v>5662</v>
+        <v>5664</v>
       </c>
       <c r="B2793" t="s">
         <v>5563</v>
@@ -83185,12 +83205,12 @@
         <v>1790</v>
       </c>
       <c r="P2793" t="s">
-        <v>5663</v>
+        <v>6596</v>
       </c>
     </row>
     <row r="2794" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2794" s="1" t="s">
-        <v>5664</v>
+        <v>5665</v>
       </c>
       <c r="B2794" t="s">
         <v>5563</v>
@@ -83205,12 +83225,12 @@
         <v>1790</v>
       </c>
       <c r="P2794" t="s">
-        <v>6596</v>
+        <v>5666</v>
       </c>
     </row>
     <row r="2795" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2795" s="1" t="s">
-        <v>5665</v>
+        <v>5667</v>
       </c>
       <c r="B2795" t="s">
         <v>5563</v>
@@ -83225,12 +83245,12 @@
         <v>1790</v>
       </c>
       <c r="P2795" t="s">
-        <v>5666</v>
+        <v>6597</v>
       </c>
     </row>
     <row r="2796" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2796" s="1" t="s">
-        <v>5667</v>
+        <v>5668</v>
       </c>
       <c r="B2796" t="s">
         <v>5563</v>
@@ -83245,12 +83265,12 @@
         <v>1790</v>
       </c>
       <c r="P2796" t="s">
-        <v>6597</v>
+        <v>6598</v>
       </c>
     </row>
     <row r="2797" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2797" s="1" t="s">
-        <v>5668</v>
+        <v>5669</v>
       </c>
       <c r="B2797" t="s">
         <v>5563</v>
@@ -83265,12 +83285,12 @@
         <v>1790</v>
       </c>
       <c r="P2797" t="s">
-        <v>6598</v>
+        <v>6599</v>
       </c>
     </row>
     <row r="2798" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2798" s="1" t="s">
-        <v>5669</v>
+        <v>5670</v>
       </c>
       <c r="B2798" t="s">
         <v>5563</v>
@@ -83285,12 +83305,12 @@
         <v>1790</v>
       </c>
       <c r="P2798" t="s">
-        <v>6599</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="2799" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2799" s="1" t="s">
-        <v>5670</v>
+        <v>5671</v>
       </c>
       <c r="B2799" t="s">
         <v>5563</v>
@@ -83305,12 +83325,12 @@
         <v>1790</v>
       </c>
       <c r="P2799" t="s">
-        <v>6600</v>
+        <v>6601</v>
       </c>
     </row>
     <row r="2800" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2800" s="1" t="s">
-        <v>5671</v>
+        <v>5672</v>
       </c>
       <c r="B2800" t="s">
         <v>5563</v>
@@ -83325,12 +83345,12 @@
         <v>1790</v>
       </c>
       <c r="P2800" t="s">
-        <v>6601</v>
+        <v>5673</v>
       </c>
     </row>
     <row r="2801" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2801" s="1" t="s">
-        <v>5672</v>
+        <v>5674</v>
       </c>
       <c r="B2801" t="s">
         <v>5563</v>
@@ -83345,12 +83365,12 @@
         <v>1790</v>
       </c>
       <c r="P2801" t="s">
-        <v>5673</v>
+        <v>6602</v>
       </c>
     </row>
     <row r="2802" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2802" s="1" t="s">
-        <v>5674</v>
+        <v>5675</v>
       </c>
       <c r="B2802" t="s">
         <v>5563</v>
@@ -83365,12 +83385,12 @@
         <v>1790</v>
       </c>
       <c r="P2802" t="s">
-        <v>6602</v>
+        <v>5676</v>
       </c>
     </row>
     <row r="2803" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2803" s="1" t="s">
-        <v>5675</v>
+        <v>5677</v>
       </c>
       <c r="B2803" t="s">
         <v>5563</v>
@@ -83385,12 +83405,12 @@
         <v>1790</v>
       </c>
       <c r="P2803" t="s">
-        <v>5676</v>
+        <v>6603</v>
       </c>
     </row>
     <row r="2804" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2804" s="1" t="s">
-        <v>5677</v>
+        <v>5678</v>
       </c>
       <c r="B2804" t="s">
         <v>5563</v>
@@ -83405,12 +83425,12 @@
         <v>1790</v>
       </c>
       <c r="P2804" t="s">
-        <v>6603</v>
+        <v>5679</v>
       </c>
     </row>
     <row r="2805" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2805" s="1" t="s">
-        <v>5678</v>
+        <v>5680</v>
       </c>
       <c r="B2805" t="s">
         <v>5563</v>
@@ -83425,12 +83445,12 @@
         <v>1790</v>
       </c>
       <c r="P2805" t="s">
-        <v>5679</v>
+        <v>5681</v>
       </c>
     </row>
     <row r="2806" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2806" s="1" t="s">
-        <v>5680</v>
+        <v>5682</v>
       </c>
       <c r="B2806" t="s">
         <v>5563</v>
@@ -83445,12 +83465,12 @@
         <v>1790</v>
       </c>
       <c r="P2806" t="s">
-        <v>5681</v>
+        <v>6604</v>
       </c>
     </row>
     <row r="2807" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2807" s="1" t="s">
-        <v>5682</v>
+        <v>5683</v>
       </c>
       <c r="B2807" t="s">
         <v>5563</v>
@@ -83465,12 +83485,12 @@
         <v>1790</v>
       </c>
       <c r="P2807" t="s">
-        <v>6604</v>
+        <v>6605</v>
       </c>
     </row>
     <row r="2808" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2808" s="1" t="s">
-        <v>5683</v>
+        <v>5684</v>
       </c>
       <c r="B2808" t="s">
         <v>5563</v>
@@ -83485,12 +83505,12 @@
         <v>1790</v>
       </c>
       <c r="P2808" t="s">
-        <v>6605</v>
+        <v>5685</v>
       </c>
     </row>
     <row r="2809" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2809" s="1" t="s">
-        <v>5684</v>
+        <v>5686</v>
       </c>
       <c r="B2809" t="s">
         <v>5563</v>
@@ -83505,12 +83525,12 @@
         <v>1790</v>
       </c>
       <c r="P2809" t="s">
-        <v>5685</v>
+        <v>5687</v>
       </c>
     </row>
     <row r="2810" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2810" s="1" t="s">
-        <v>5686</v>
+        <v>5688</v>
       </c>
       <c r="B2810" t="s">
         <v>5563</v>
@@ -83525,12 +83545,12 @@
         <v>1790</v>
       </c>
       <c r="P2810" t="s">
-        <v>5687</v>
+        <v>6606</v>
       </c>
     </row>
     <row r="2811" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2811" s="1" t="s">
-        <v>5688</v>
+        <v>5689</v>
       </c>
       <c r="B2811" t="s">
         <v>5563</v>
@@ -83545,12 +83565,12 @@
         <v>1790</v>
       </c>
       <c r="P2811" t="s">
-        <v>6606</v>
+        <v>5690</v>
       </c>
     </row>
     <row r="2812" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2812" s="1" t="s">
-        <v>5689</v>
+        <v>5691</v>
       </c>
       <c r="B2812" t="s">
         <v>5563</v>
@@ -83565,12 +83585,12 @@
         <v>1790</v>
       </c>
       <c r="P2812" t="s">
-        <v>5690</v>
+        <v>6607</v>
       </c>
     </row>
     <row r="2813" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2813" s="1" t="s">
-        <v>5691</v>
+        <v>5692</v>
       </c>
       <c r="B2813" t="s">
         <v>5563</v>
@@ -83585,12 +83605,12 @@
         <v>1790</v>
       </c>
       <c r="P2813" t="s">
-        <v>6607</v>
+        <v>6608</v>
       </c>
     </row>
     <row r="2814" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2814" s="1" t="s">
-        <v>5692</v>
+        <v>5693</v>
       </c>
       <c r="B2814" t="s">
         <v>5563</v>
@@ -83605,12 +83625,12 @@
         <v>1790</v>
       </c>
       <c r="P2814" t="s">
-        <v>6608</v>
+        <v>6609</v>
       </c>
     </row>
     <row r="2815" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2815" s="1" t="s">
-        <v>5693</v>
+        <v>5694</v>
       </c>
       <c r="B2815" t="s">
         <v>5563</v>
@@ -83625,12 +83645,12 @@
         <v>1790</v>
       </c>
       <c r="P2815" t="s">
-        <v>6609</v>
+        <v>6610</v>
       </c>
     </row>
     <row r="2816" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2816" s="1" t="s">
-        <v>5694</v>
+        <v>5695</v>
       </c>
       <c r="B2816" t="s">
         <v>5563</v>
@@ -83645,12 +83665,12 @@
         <v>1790</v>
       </c>
       <c r="P2816" t="s">
-        <v>6610</v>
+        <v>6611</v>
       </c>
     </row>
     <row r="2817" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2817" s="1" t="s">
-        <v>5695</v>
+        <v>5696</v>
       </c>
       <c r="B2817" t="s">
         <v>5563</v>
@@ -83665,12 +83685,12 @@
         <v>1790</v>
       </c>
       <c r="P2817" t="s">
-        <v>6611</v>
+        <v>6612</v>
       </c>
     </row>
     <row r="2818" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2818" s="1" t="s">
-        <v>5696</v>
+        <v>5697</v>
       </c>
       <c r="B2818" t="s">
         <v>5563</v>
@@ -83685,12 +83705,12 @@
         <v>1790</v>
       </c>
       <c r="P2818" t="s">
-        <v>6612</v>
+        <v>5698</v>
       </c>
     </row>
     <row r="2819" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2819" s="1" t="s">
-        <v>5697</v>
+        <v>5699</v>
       </c>
       <c r="B2819" t="s">
         <v>5563</v>
@@ -83705,12 +83725,12 @@
         <v>1790</v>
       </c>
       <c r="P2819" t="s">
-        <v>5698</v>
+        <v>6613</v>
       </c>
     </row>
     <row r="2820" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2820" s="1" t="s">
-        <v>5699</v>
+        <v>5700</v>
       </c>
       <c r="B2820" t="s">
         <v>5563</v>
@@ -83725,12 +83745,12 @@
         <v>1790</v>
       </c>
       <c r="P2820" t="s">
-        <v>6613</v>
+        <v>6614</v>
       </c>
     </row>
     <row r="2821" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2821" s="1" t="s">
-        <v>5700</v>
+        <v>5701</v>
       </c>
       <c r="B2821" t="s">
         <v>5563</v>
@@ -83745,12 +83765,12 @@
         <v>1790</v>
       </c>
       <c r="P2821" t="s">
-        <v>6614</v>
+        <v>5702</v>
       </c>
     </row>
     <row r="2822" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2822" s="1" t="s">
-        <v>5701</v>
+        <v>5703</v>
       </c>
       <c r="B2822" t="s">
         <v>5563</v>
@@ -83765,12 +83785,12 @@
         <v>1790</v>
       </c>
       <c r="P2822" t="s">
-        <v>5702</v>
+        <v>6615</v>
       </c>
     </row>
     <row r="2823" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2823" s="1" t="s">
-        <v>5703</v>
+        <v>5704</v>
       </c>
       <c r="B2823" t="s">
         <v>5563</v>
@@ -83785,12 +83805,12 @@
         <v>1790</v>
       </c>
       <c r="P2823" t="s">
-        <v>6615</v>
+        <v>5705</v>
       </c>
     </row>
     <row r="2824" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2824" s="1" t="s">
-        <v>5704</v>
+        <v>5706</v>
       </c>
       <c r="B2824" t="s">
         <v>5563</v>
@@ -83805,12 +83825,12 @@
         <v>1790</v>
       </c>
       <c r="P2824" t="s">
-        <v>5705</v>
+        <v>5707</v>
       </c>
     </row>
     <row r="2825" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2825" s="1" t="s">
-        <v>5706</v>
+        <v>5708</v>
       </c>
       <c r="B2825" t="s">
         <v>5563</v>
@@ -83825,12 +83845,12 @@
         <v>1790</v>
       </c>
       <c r="P2825" t="s">
-        <v>5707</v>
+        <v>6616</v>
       </c>
     </row>
     <row r="2826" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2826" s="1" t="s">
-        <v>5708</v>
+        <v>5709</v>
       </c>
       <c r="B2826" t="s">
         <v>5563</v>
@@ -83845,12 +83865,12 @@
         <v>1790</v>
       </c>
       <c r="P2826" t="s">
-        <v>6616</v>
+        <v>5710</v>
       </c>
     </row>
     <row r="2827" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2827" s="1" t="s">
-        <v>5709</v>
+        <v>5711</v>
       </c>
       <c r="B2827" t="s">
         <v>5563</v>
@@ -83865,12 +83885,12 @@
         <v>1790</v>
       </c>
       <c r="P2827" t="s">
-        <v>5710</v>
+        <v>6617</v>
       </c>
     </row>
     <row r="2828" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2828" s="1" t="s">
-        <v>5711</v>
+        <v>5712</v>
       </c>
       <c r="B2828" t="s">
         <v>5563</v>
@@ -83885,12 +83905,12 @@
         <v>1790</v>
       </c>
       <c r="P2828" t="s">
-        <v>6617</v>
+        <v>6618</v>
       </c>
     </row>
     <row r="2829" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2829" s="1" t="s">
-        <v>5712</v>
+        <v>5713</v>
       </c>
       <c r="B2829" t="s">
         <v>5563</v>
@@ -83905,12 +83925,12 @@
         <v>1790</v>
       </c>
       <c r="P2829" t="s">
-        <v>6618</v>
+        <v>6619</v>
       </c>
     </row>
     <row r="2830" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2830" s="1" t="s">
-        <v>5713</v>
+        <v>5714</v>
       </c>
       <c r="B2830" t="s">
         <v>5563</v>
@@ -83925,12 +83945,12 @@
         <v>1790</v>
       </c>
       <c r="P2830" t="s">
-        <v>6619</v>
+        <v>6620</v>
       </c>
     </row>
     <row r="2831" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2831" s="1" t="s">
-        <v>5714</v>
+        <v>5715</v>
       </c>
       <c r="B2831" t="s">
         <v>5563</v>
@@ -83945,12 +83965,12 @@
         <v>1790</v>
       </c>
       <c r="P2831" t="s">
-        <v>6620</v>
+        <v>6621</v>
       </c>
     </row>
     <row r="2832" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2832" s="1" t="s">
-        <v>5715</v>
+        <v>5716</v>
       </c>
       <c r="B2832" t="s">
         <v>5563</v>
@@ -83965,12 +83985,12 @@
         <v>1790</v>
       </c>
       <c r="P2832" t="s">
-        <v>6621</v>
+        <v>5717</v>
       </c>
     </row>
     <row r="2833" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2833" s="1" t="s">
-        <v>5716</v>
+        <v>5718</v>
       </c>
       <c r="B2833" t="s">
         <v>5563</v>
@@ -83985,12 +84005,12 @@
         <v>1790</v>
       </c>
       <c r="P2833" t="s">
-        <v>5717</v>
+        <v>6622</v>
       </c>
     </row>
     <row r="2834" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2834" s="1" t="s">
-        <v>5718</v>
+        <v>5719</v>
       </c>
       <c r="B2834" t="s">
         <v>5563</v>
@@ -84005,12 +84025,12 @@
         <v>1790</v>
       </c>
       <c r="P2834" t="s">
-        <v>6622</v>
+        <v>6623</v>
       </c>
     </row>
     <row r="2835" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2835" s="1" t="s">
-        <v>5719</v>
+        <v>5720</v>
       </c>
       <c r="B2835" t="s">
         <v>5563</v>
@@ -84025,12 +84045,12 @@
         <v>1790</v>
       </c>
       <c r="P2835" t="s">
-        <v>6623</v>
+        <v>5721</v>
       </c>
     </row>
     <row r="2836" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2836" s="1" t="s">
-        <v>5720</v>
+        <v>5722</v>
       </c>
       <c r="B2836" t="s">
         <v>5563</v>
@@ -84045,12 +84065,12 @@
         <v>1790</v>
       </c>
       <c r="P2836" t="s">
-        <v>5721</v>
+        <v>5723</v>
       </c>
     </row>
     <row r="2837" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2837" s="1" t="s">
-        <v>5722</v>
+        <v>5724</v>
       </c>
       <c r="B2837" t="s">
         <v>5563</v>
@@ -84065,12 +84085,12 @@
         <v>1790</v>
       </c>
       <c r="P2837" t="s">
-        <v>5723</v>
+        <v>5725</v>
       </c>
     </row>
     <row r="2838" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2838" s="1" t="s">
-        <v>5724</v>
+        <v>5726</v>
       </c>
       <c r="B2838" t="s">
         <v>5563</v>
@@ -84085,12 +84105,12 @@
         <v>1790</v>
       </c>
       <c r="P2838" t="s">
-        <v>5725</v>
+        <v>5727</v>
       </c>
     </row>
     <row r="2839" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2839" s="1" t="s">
-        <v>5726</v>
+        <v>5728</v>
       </c>
       <c r="B2839" t="s">
         <v>5563</v>
@@ -84105,12 +84125,12 @@
         <v>1790</v>
       </c>
       <c r="P2839" t="s">
-        <v>5727</v>
+        <v>6624</v>
       </c>
     </row>
     <row r="2840" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2840" s="1" t="s">
-        <v>5728</v>
+        <v>5729</v>
       </c>
       <c r="B2840" t="s">
         <v>5563</v>
@@ -84125,12 +84145,12 @@
         <v>1790</v>
       </c>
       <c r="P2840" t="s">
-        <v>6624</v>
+        <v>5730</v>
       </c>
     </row>
     <row r="2841" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2841" s="1" t="s">
-        <v>5729</v>
+        <v>5731</v>
       </c>
       <c r="B2841" t="s">
         <v>5563</v>
@@ -84145,12 +84165,12 @@
         <v>1790</v>
       </c>
       <c r="P2841" t="s">
-        <v>5730</v>
+        <v>5732</v>
       </c>
     </row>
     <row r="2842" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2842" s="1" t="s">
-        <v>5731</v>
+        <v>5733</v>
       </c>
       <c r="B2842" t="s">
         <v>5563</v>
@@ -84165,12 +84185,12 @@
         <v>1790</v>
       </c>
       <c r="P2842" t="s">
-        <v>5732</v>
+        <v>6625</v>
       </c>
     </row>
     <row r="2843" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2843" s="1" t="s">
-        <v>5733</v>
+        <v>5734</v>
       </c>
       <c r="B2843" t="s">
         <v>5563</v>
@@ -84185,12 +84205,12 @@
         <v>1790</v>
       </c>
       <c r="P2843" t="s">
-        <v>6625</v>
+        <v>5735</v>
       </c>
     </row>
     <row r="2844" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2844" s="1" t="s">
-        <v>5734</v>
+        <v>5736</v>
       </c>
       <c r="B2844" t="s">
         <v>5563</v>
@@ -84205,12 +84225,12 @@
         <v>1790</v>
       </c>
       <c r="P2844" t="s">
-        <v>5735</v>
+        <v>6626</v>
       </c>
     </row>
     <row r="2845" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2845" s="1" t="s">
-        <v>5736</v>
+        <v>5737</v>
       </c>
       <c r="B2845" t="s">
         <v>5563</v>
@@ -84225,12 +84245,12 @@
         <v>1790</v>
       </c>
       <c r="P2845" t="s">
-        <v>6626</v>
+        <v>5738</v>
       </c>
     </row>
     <row r="2846" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2846" s="1" t="s">
-        <v>5737</v>
+        <v>5739</v>
       </c>
       <c r="B2846" t="s">
         <v>5563</v>
@@ -84245,12 +84265,12 @@
         <v>1790</v>
       </c>
       <c r="P2846" t="s">
-        <v>5738</v>
+        <v>5740</v>
       </c>
     </row>
     <row r="2847" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2847" s="1" t="s">
-        <v>5739</v>
+        <v>5741</v>
       </c>
       <c r="B2847" t="s">
         <v>5563</v>
@@ -84265,12 +84285,12 @@
         <v>1790</v>
       </c>
       <c r="P2847" t="s">
-        <v>5740</v>
+        <v>5742</v>
       </c>
     </row>
     <row r="2848" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2848" s="1" t="s">
-        <v>5741</v>
+        <v>5743</v>
       </c>
       <c r="B2848" t="s">
         <v>5563</v>
@@ -84285,12 +84305,12 @@
         <v>1790</v>
       </c>
       <c r="P2848" t="s">
-        <v>5742</v>
+        <v>5744</v>
       </c>
     </row>
     <row r="2849" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2849" s="1" t="s">
-        <v>5743</v>
+        <v>5745</v>
       </c>
       <c r="B2849" t="s">
         <v>5563</v>
@@ -84305,12 +84325,12 @@
         <v>1790</v>
       </c>
       <c r="P2849" t="s">
-        <v>5744</v>
+        <v>6627</v>
       </c>
     </row>
     <row r="2850" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2850" s="1" t="s">
-        <v>5745</v>
+        <v>5746</v>
       </c>
       <c r="B2850" t="s">
         <v>5563</v>
@@ -84325,12 +84345,12 @@
         <v>1790</v>
       </c>
       <c r="P2850" t="s">
-        <v>6627</v>
+        <v>6628</v>
       </c>
     </row>
     <row r="2851" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2851" s="1" t="s">
-        <v>5746</v>
+        <v>5747</v>
       </c>
       <c r="B2851" t="s">
         <v>5563</v>
@@ -84345,12 +84365,12 @@
         <v>1790</v>
       </c>
       <c r="P2851" t="s">
-        <v>6628</v>
+        <v>6629</v>
       </c>
     </row>
     <row r="2852" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2852" s="1" t="s">
-        <v>5747</v>
+        <v>5748</v>
       </c>
       <c r="B2852" t="s">
         <v>5563</v>
@@ -84365,12 +84385,12 @@
         <v>1790</v>
       </c>
       <c r="P2852" t="s">
-        <v>6629</v>
+        <v>6630</v>
       </c>
     </row>
     <row r="2853" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2853" s="1" t="s">
-        <v>5748</v>
+        <v>5749</v>
       </c>
       <c r="B2853" t="s">
         <v>5563</v>
@@ -84385,12 +84405,12 @@
         <v>1790</v>
       </c>
       <c r="P2853" t="s">
-        <v>6630</v>
+        <v>6631</v>
       </c>
     </row>
     <row r="2854" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2854" s="1" t="s">
-        <v>5749</v>
+        <v>5750</v>
       </c>
       <c r="B2854" t="s">
         <v>5563</v>
@@ -84405,12 +84425,12 @@
         <v>1790</v>
       </c>
       <c r="P2854" t="s">
-        <v>6631</v>
+        <v>5751</v>
       </c>
     </row>
     <row r="2855" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2855" s="1" t="s">
-        <v>5750</v>
+        <v>5752</v>
       </c>
       <c r="B2855" t="s">
         <v>5563</v>
@@ -84425,12 +84445,12 @@
         <v>1790</v>
       </c>
       <c r="P2855" t="s">
-        <v>5751</v>
+        <v>6632</v>
       </c>
     </row>
     <row r="2856" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2856" s="1" t="s">
-        <v>5752</v>
+        <v>5753</v>
       </c>
       <c r="B2856" t="s">
         <v>5563</v>
@@ -84445,12 +84465,12 @@
         <v>1790</v>
       </c>
       <c r="P2856" t="s">
-        <v>6632</v>
+        <v>5754</v>
       </c>
     </row>
     <row r="2857" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2857" s="1" t="s">
-        <v>5753</v>
+        <v>5755</v>
       </c>
       <c r="B2857" t="s">
         <v>5563</v>
@@ -84465,12 +84485,12 @@
         <v>1790</v>
       </c>
       <c r="P2857" t="s">
-        <v>5754</v>
+        <v>6633</v>
       </c>
     </row>
     <row r="2858" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2858" s="1" t="s">
-        <v>5755</v>
+        <v>5756</v>
       </c>
       <c r="B2858" t="s">
         <v>5563</v>
@@ -84485,12 +84505,12 @@
         <v>1790</v>
       </c>
       <c r="P2858" t="s">
-        <v>6633</v>
+        <v>5757</v>
       </c>
     </row>
     <row r="2859" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2859" s="1" t="s">
-        <v>5756</v>
+        <v>5758</v>
       </c>
       <c r="B2859" t="s">
         <v>5563</v>
@@ -84505,12 +84525,12 @@
         <v>1790</v>
       </c>
       <c r="P2859" t="s">
-        <v>5757</v>
+        <v>6634</v>
       </c>
     </row>
     <row r="2860" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2860" s="1" t="s">
-        <v>5758</v>
+        <v>5759</v>
       </c>
       <c r="B2860" t="s">
         <v>5563</v>
@@ -84525,12 +84545,12 @@
         <v>1790</v>
       </c>
       <c r="P2860" t="s">
-        <v>6634</v>
+        <v>6635</v>
       </c>
     </row>
     <row r="2861" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2861" s="1" t="s">
-        <v>5759</v>
+        <v>5760</v>
       </c>
       <c r="B2861" t="s">
         <v>5563</v>
@@ -84545,12 +84565,12 @@
         <v>1790</v>
       </c>
       <c r="P2861" t="s">
-        <v>6635</v>
+        <v>6636</v>
       </c>
     </row>
     <row r="2862" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2862" s="1" t="s">
-        <v>5760</v>
+        <v>5761</v>
       </c>
       <c r="B2862" t="s">
         <v>5563</v>
@@ -84565,26 +84585,6 @@
         <v>1790</v>
       </c>
       <c r="P2862" t="s">
-        <v>6636</v>
-      </c>
-    </row>
-    <row r="2863" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2863" s="1" t="s">
-        <v>5761</v>
-      </c>
-      <c r="B2863" t="s">
-        <v>5563</v>
-      </c>
-      <c r="C2863">
-        <v>68000</v>
-      </c>
-      <c r="D2863" t="s">
-        <v>168</v>
-      </c>
-      <c r="K2863" t="s">
-        <v>1790</v>
-      </c>
-      <c r="P2863" t="s">
         <v>6637</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added working gotya driver
</commit_message>
<xml_diff>
--- a/emulator/compatibility_list.xlsx
+++ b/emulator/compatibility_list.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Φύλλο2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="OUT___Αντιγραφή" localSheetId="2">Φύλλο2!$A$1:$P$2862</definedName>
+    <definedName name="OUT___Αντιγραφή" localSheetId="2">Φύλλο2!$A$1:$P$2861</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20299,10 +20299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R142"/>
+  <dimension ref="A1:R143"/>
   <sheetViews>
     <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+      <selection activeCell="A143" sqref="A143:XFD143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23128,6 +23128,23 @@
       </c>
       <c r="P142" t="s">
         <v>5490</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>5528</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5529</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+      <c r="K143" t="s">
+        <v>537</v>
+      </c>
+      <c r="P143" t="s">
+        <v>6564</v>
       </c>
     </row>
   </sheetData>
@@ -23245,10 +23262,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2862"/>
+  <dimension ref="A1:P2861"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2686" workbookViewId="0">
-      <selection activeCell="A2701" sqref="A2701:XFD2701"/>
+      <selection activeCell="A2714" sqref="A2714:XFD2714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -81634,24 +81651,24 @@
     </row>
     <row r="2714" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2714" s="1" t="s">
-        <v>5528</v>
+        <v>5530</v>
       </c>
       <c r="B2714" t="s">
-        <v>5529</v>
+        <v>5531</v>
       </c>
       <c r="C2714" t="s">
         <v>2</v>
       </c>
       <c r="K2714" t="s">
-        <v>537</v>
+        <v>63</v>
       </c>
       <c r="P2714" t="s">
-        <v>6564</v>
+        <v>5532</v>
       </c>
     </row>
     <row r="2715" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2715" s="1" t="s">
-        <v>5530</v>
+        <v>5533</v>
       </c>
       <c r="B2715" t="s">
         <v>5531</v>
@@ -81663,80 +81680,83 @@
         <v>63</v>
       </c>
       <c r="P2715" t="s">
-        <v>5532</v>
+        <v>5534</v>
       </c>
     </row>
     <row r="2716" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2716" s="1" t="s">
-        <v>5533</v>
+        <v>5535</v>
       </c>
       <c r="B2716" t="s">
-        <v>5531</v>
+        <v>5536</v>
       </c>
       <c r="C2716" t="s">
         <v>2</v>
       </c>
       <c r="K2716" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="P2716" t="s">
-        <v>5534</v>
+        <v>5537</v>
       </c>
     </row>
     <row r="2717" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2717" s="1" t="s">
-        <v>5535</v>
+        <v>5538</v>
       </c>
       <c r="B2717" t="s">
-        <v>5536</v>
+        <v>5539</v>
       </c>
       <c r="C2717" t="s">
         <v>2</v>
       </c>
       <c r="K2717" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="P2717" t="s">
-        <v>5537</v>
+        <v>5540</v>
       </c>
     </row>
     <row r="2718" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2718" s="1" t="s">
-        <v>5538</v>
+        <v>5541</v>
       </c>
       <c r="B2718" t="s">
-        <v>5539</v>
+        <v>5542</v>
       </c>
       <c r="C2718" t="s">
         <v>2</v>
       </c>
       <c r="K2718" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="P2718" t="s">
-        <v>5540</v>
+        <v>5543</v>
       </c>
     </row>
     <row r="2719" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2719" s="1" t="s">
-        <v>5541</v>
+        <v>5544</v>
       </c>
       <c r="B2719" t="s">
-        <v>5542</v>
+        <v>5545</v>
       </c>
       <c r="C2719" t="s">
         <v>2</v>
       </c>
+      <c r="D2719" t="s">
+        <v>2</v>
+      </c>
       <c r="K2719" t="s">
-        <v>60</v>
+        <v>693</v>
       </c>
       <c r="P2719" t="s">
-        <v>5543</v>
+        <v>6565</v>
       </c>
     </row>
     <row r="2720" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2720" s="1" t="s">
-        <v>5544</v>
+        <v>5546</v>
       </c>
       <c r="B2720" t="s">
         <v>5545</v>
@@ -81751,32 +81771,29 @@
         <v>693</v>
       </c>
       <c r="P2720" t="s">
-        <v>6565</v>
+        <v>6566</v>
       </c>
     </row>
     <row r="2721" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2721" s="1" t="s">
-        <v>5546</v>
+        <v>5547</v>
       </c>
       <c r="B2721" t="s">
-        <v>5545</v>
+        <v>5548</v>
       </c>
       <c r="C2721" t="s">
         <v>2</v>
       </c>
-      <c r="D2721" t="s">
-        <v>2</v>
-      </c>
       <c r="K2721" t="s">
-        <v>693</v>
+        <v>60</v>
       </c>
       <c r="P2721" t="s">
-        <v>6566</v>
+        <v>5549</v>
       </c>
     </row>
     <row r="2722" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2722" s="1" t="s">
-        <v>5547</v>
+        <v>5550</v>
       </c>
       <c r="B2722" t="s">
         <v>5548</v>
@@ -81784,16 +81801,25 @@
       <c r="C2722" t="s">
         <v>2</v>
       </c>
+      <c r="D2722" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2722" t="s">
+        <v>168</v>
+      </c>
       <c r="K2722" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2722" t="s">
         <v>60</v>
       </c>
       <c r="P2722" t="s">
-        <v>5549</v>
+        <v>5551</v>
       </c>
     </row>
     <row r="2723" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2723" s="1" t="s">
-        <v>5550</v>
+        <v>5552</v>
       </c>
       <c r="B2723" t="s">
         <v>5548</v>
@@ -81814,55 +81840,43 @@
         <v>60</v>
       </c>
       <c r="P2723" t="s">
-        <v>5551</v>
+        <v>5553</v>
       </c>
     </row>
     <row r="2724" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2724" s="1" t="s">
-        <v>5552</v>
+        <v>5554</v>
       </c>
       <c r="B2724" t="s">
-        <v>5548</v>
-      </c>
-      <c r="C2724" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2724" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2724" t="s">
-        <v>168</v>
+        <v>5555</v>
+      </c>
+      <c r="C2724">
+        <v>68000</v>
       </c>
       <c r="K2724" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2724" t="s">
-        <v>60</v>
+        <v>2076</v>
       </c>
       <c r="P2724" t="s">
-        <v>5553</v>
+        <v>5556</v>
       </c>
     </row>
     <row r="2725" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2725" s="1" t="s">
-        <v>5554</v>
+        <v>5557</v>
       </c>
       <c r="B2725" t="s">
-        <v>5555</v>
-      </c>
-      <c r="C2725">
-        <v>68000</v>
-      </c>
-      <c r="K2725" t="s">
-        <v>2076</v>
+        <v>5558</v>
+      </c>
+      <c r="C2725" t="s">
+        <v>2</v>
       </c>
       <c r="P2725" t="s">
-        <v>5556</v>
+        <v>5559</v>
       </c>
     </row>
     <row r="2726" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2726" s="1" t="s">
-        <v>5557</v>
+        <v>5560</v>
       </c>
       <c r="B2726" t="s">
         <v>5558</v>
@@ -81871,26 +81885,32 @@
         <v>2</v>
       </c>
       <c r="P2726" t="s">
-        <v>5559</v>
+        <v>5561</v>
       </c>
     </row>
     <row r="2727" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2727" s="1" t="s">
-        <v>5560</v>
+        <v>5562</v>
       </c>
       <c r="B2727" t="s">
-        <v>5558</v>
-      </c>
-      <c r="C2727" t="s">
-        <v>2</v>
+        <v>5563</v>
+      </c>
+      <c r="C2727">
+        <v>68000</v>
+      </c>
+      <c r="D2727" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2727" t="s">
+        <v>1790</v>
       </c>
       <c r="P2727" t="s">
-        <v>5561</v>
+        <v>5564</v>
       </c>
     </row>
     <row r="2728" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2728" s="1" t="s">
-        <v>5562</v>
+        <v>5565</v>
       </c>
       <c r="B2728" t="s">
         <v>5563</v>
@@ -81905,12 +81925,12 @@
         <v>1790</v>
       </c>
       <c r="P2728" t="s">
-        <v>5564</v>
+        <v>6567</v>
       </c>
     </row>
     <row r="2729" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2729" s="1" t="s">
-        <v>5565</v>
+        <v>5566</v>
       </c>
       <c r="B2729" t="s">
         <v>5563</v>
@@ -81925,12 +81945,12 @@
         <v>1790</v>
       </c>
       <c r="P2729" t="s">
-        <v>6567</v>
+        <v>5567</v>
       </c>
     </row>
     <row r="2730" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2730" s="1" t="s">
-        <v>5566</v>
+        <v>5568</v>
       </c>
       <c r="B2730" t="s">
         <v>5563</v>
@@ -81945,12 +81965,12 @@
         <v>1790</v>
       </c>
       <c r="P2730" t="s">
-        <v>5567</v>
+        <v>5569</v>
       </c>
     </row>
     <row r="2731" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2731" s="1" t="s">
-        <v>5568</v>
+        <v>5570</v>
       </c>
       <c r="B2731" t="s">
         <v>5563</v>
@@ -81965,12 +81985,12 @@
         <v>1790</v>
       </c>
       <c r="P2731" t="s">
-        <v>5569</v>
+        <v>5571</v>
       </c>
     </row>
     <row r="2732" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2732" s="1" t="s">
-        <v>5570</v>
+        <v>5572</v>
       </c>
       <c r="B2732" t="s">
         <v>5563</v>
@@ -81985,12 +82005,12 @@
         <v>1790</v>
       </c>
       <c r="P2732" t="s">
-        <v>5571</v>
+        <v>5573</v>
       </c>
     </row>
     <row r="2733" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2733" s="1" t="s">
-        <v>5572</v>
+        <v>5574</v>
       </c>
       <c r="B2733" t="s">
         <v>5563</v>
@@ -82005,12 +82025,12 @@
         <v>1790</v>
       </c>
       <c r="P2733" t="s">
-        <v>5573</v>
+        <v>5575</v>
       </c>
     </row>
     <row r="2734" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2734" s="1" t="s">
-        <v>5574</v>
+        <v>5576</v>
       </c>
       <c r="B2734" t="s">
         <v>5563</v>
@@ -82025,12 +82045,12 @@
         <v>1790</v>
       </c>
       <c r="P2734" t="s">
-        <v>5575</v>
+        <v>5577</v>
       </c>
     </row>
     <row r="2735" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2735" s="1" t="s">
-        <v>5576</v>
+        <v>5578</v>
       </c>
       <c r="B2735" t="s">
         <v>5563</v>
@@ -82045,12 +82065,12 @@
         <v>1790</v>
       </c>
       <c r="P2735" t="s">
-        <v>5577</v>
+        <v>6568</v>
       </c>
     </row>
     <row r="2736" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2736" s="1" t="s">
-        <v>5578</v>
+        <v>5579</v>
       </c>
       <c r="B2736" t="s">
         <v>5563</v>
@@ -82065,12 +82085,12 @@
         <v>1790</v>
       </c>
       <c r="P2736" t="s">
-        <v>6568</v>
+        <v>5580</v>
       </c>
     </row>
     <row r="2737" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2737" s="1" t="s">
-        <v>5579</v>
+        <v>5581</v>
       </c>
       <c r="B2737" t="s">
         <v>5563</v>
@@ -82085,12 +82105,12 @@
         <v>1790</v>
       </c>
       <c r="P2737" t="s">
-        <v>5580</v>
+        <v>5582</v>
       </c>
     </row>
     <row r="2738" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2738" s="1" t="s">
-        <v>5581</v>
+        <v>5583</v>
       </c>
       <c r="B2738" t="s">
         <v>5563</v>
@@ -82105,12 +82125,12 @@
         <v>1790</v>
       </c>
       <c r="P2738" t="s">
-        <v>5582</v>
+        <v>5584</v>
       </c>
     </row>
     <row r="2739" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2739" s="1" t="s">
-        <v>5583</v>
+        <v>5585</v>
       </c>
       <c r="B2739" t="s">
         <v>5563</v>
@@ -82125,12 +82145,12 @@
         <v>1790</v>
       </c>
       <c r="P2739" t="s">
-        <v>5584</v>
+        <v>5586</v>
       </c>
     </row>
     <row r="2740" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2740" s="1" t="s">
-        <v>5585</v>
+        <v>5587</v>
       </c>
       <c r="B2740" t="s">
         <v>5563</v>
@@ -82145,12 +82165,12 @@
         <v>1790</v>
       </c>
       <c r="P2740" t="s">
-        <v>5586</v>
+        <v>5588</v>
       </c>
     </row>
     <row r="2741" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2741" s="1" t="s">
-        <v>5587</v>
+        <v>5589</v>
       </c>
       <c r="B2741" t="s">
         <v>5563</v>
@@ -82165,12 +82185,12 @@
         <v>1790</v>
       </c>
       <c r="P2741" t="s">
-        <v>5588</v>
+        <v>6569</v>
       </c>
     </row>
     <row r="2742" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2742" s="1" t="s">
-        <v>5589</v>
+        <v>5590</v>
       </c>
       <c r="B2742" t="s">
         <v>5563</v>
@@ -82185,12 +82205,12 @@
         <v>1790</v>
       </c>
       <c r="P2742" t="s">
-        <v>6569</v>
+        <v>6570</v>
       </c>
     </row>
     <row r="2743" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2743" s="1" t="s">
-        <v>5590</v>
+        <v>5591</v>
       </c>
       <c r="B2743" t="s">
         <v>5563</v>
@@ -82205,12 +82225,12 @@
         <v>1790</v>
       </c>
       <c r="P2743" t="s">
-        <v>6570</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="2744" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2744" s="1" t="s">
-        <v>5591</v>
+        <v>5593</v>
       </c>
       <c r="B2744" t="s">
         <v>5563</v>
@@ -82225,12 +82245,12 @@
         <v>1790</v>
       </c>
       <c r="P2744" t="s">
-        <v>5592</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="2745" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2745" s="1" t="s">
-        <v>5593</v>
+        <v>5595</v>
       </c>
       <c r="B2745" t="s">
         <v>5563</v>
@@ -82245,12 +82265,12 @@
         <v>1790</v>
       </c>
       <c r="P2745" t="s">
-        <v>5594</v>
+        <v>5596</v>
       </c>
     </row>
     <row r="2746" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2746" s="1" t="s">
-        <v>5595</v>
+        <v>5597</v>
       </c>
       <c r="B2746" t="s">
         <v>5563</v>
@@ -82265,12 +82285,12 @@
         <v>1790</v>
       </c>
       <c r="P2746" t="s">
-        <v>5596</v>
+        <v>5598</v>
       </c>
     </row>
     <row r="2747" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2747" s="1" t="s">
-        <v>5597</v>
+        <v>5599</v>
       </c>
       <c r="B2747" t="s">
         <v>5563</v>
@@ -82285,12 +82305,12 @@
         <v>1790</v>
       </c>
       <c r="P2747" t="s">
-        <v>5598</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="2748" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2748" s="1" t="s">
-        <v>5599</v>
+        <v>5601</v>
       </c>
       <c r="B2748" t="s">
         <v>5563</v>
@@ -82305,12 +82325,12 @@
         <v>1790</v>
       </c>
       <c r="P2748" t="s">
-        <v>5600</v>
+        <v>5602</v>
       </c>
     </row>
     <row r="2749" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2749" s="1" t="s">
-        <v>5601</v>
+        <v>5603</v>
       </c>
       <c r="B2749" t="s">
         <v>5563</v>
@@ -82325,12 +82345,12 @@
         <v>1790</v>
       </c>
       <c r="P2749" t="s">
-        <v>5602</v>
+        <v>6571</v>
       </c>
     </row>
     <row r="2750" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2750" s="1" t="s">
-        <v>5603</v>
+        <v>5604</v>
       </c>
       <c r="B2750" t="s">
         <v>5563</v>
@@ -82345,12 +82365,12 @@
         <v>1790</v>
       </c>
       <c r="P2750" t="s">
-        <v>6571</v>
+        <v>5605</v>
       </c>
     </row>
     <row r="2751" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2751" s="1" t="s">
-        <v>5604</v>
+        <v>5606</v>
       </c>
       <c r="B2751" t="s">
         <v>5563</v>
@@ -82365,12 +82385,12 @@
         <v>1790</v>
       </c>
       <c r="P2751" t="s">
-        <v>5605</v>
+        <v>5607</v>
       </c>
     </row>
     <row r="2752" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2752" s="1" t="s">
-        <v>5606</v>
+        <v>5608</v>
       </c>
       <c r="B2752" t="s">
         <v>5563</v>
@@ -82385,12 +82405,12 @@
         <v>1790</v>
       </c>
       <c r="P2752" t="s">
-        <v>5607</v>
+        <v>5609</v>
       </c>
     </row>
     <row r="2753" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2753" s="1" t="s">
-        <v>5608</v>
+        <v>5610</v>
       </c>
       <c r="B2753" t="s">
         <v>5563</v>
@@ -82405,12 +82425,12 @@
         <v>1790</v>
       </c>
       <c r="P2753" t="s">
-        <v>5609</v>
+        <v>6572</v>
       </c>
     </row>
     <row r="2754" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2754" s="1" t="s">
-        <v>5610</v>
+        <v>5611</v>
       </c>
       <c r="B2754" t="s">
         <v>5563</v>
@@ -82425,12 +82445,12 @@
         <v>1790</v>
       </c>
       <c r="P2754" t="s">
-        <v>6572</v>
+        <v>6573</v>
       </c>
     </row>
     <row r="2755" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2755" s="1" t="s">
-        <v>5611</v>
+        <v>5612</v>
       </c>
       <c r="B2755" t="s">
         <v>5563</v>
@@ -82445,12 +82465,12 @@
         <v>1790</v>
       </c>
       <c r="P2755" t="s">
-        <v>6573</v>
+        <v>6574</v>
       </c>
     </row>
     <row r="2756" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2756" s="1" t="s">
-        <v>5612</v>
+        <v>5613</v>
       </c>
       <c r="B2756" t="s">
         <v>5563</v>
@@ -82465,12 +82485,12 @@
         <v>1790</v>
       </c>
       <c r="P2756" t="s">
-        <v>6574</v>
+        <v>5614</v>
       </c>
     </row>
     <row r="2757" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2757" s="1" t="s">
-        <v>5613</v>
+        <v>5615</v>
       </c>
       <c r="B2757" t="s">
         <v>5563</v>
@@ -82485,12 +82505,12 @@
         <v>1790</v>
       </c>
       <c r="P2757" t="s">
-        <v>5614</v>
+        <v>5616</v>
       </c>
     </row>
     <row r="2758" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2758" s="1" t="s">
-        <v>5615</v>
+        <v>5617</v>
       </c>
       <c r="B2758" t="s">
         <v>5563</v>
@@ -82505,12 +82525,12 @@
         <v>1790</v>
       </c>
       <c r="P2758" t="s">
-        <v>5616</v>
+        <v>6575</v>
       </c>
     </row>
     <row r="2759" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2759" s="1" t="s">
-        <v>5617</v>
+        <v>5618</v>
       </c>
       <c r="B2759" t="s">
         <v>5563</v>
@@ -82525,12 +82545,12 @@
         <v>1790</v>
       </c>
       <c r="P2759" t="s">
-        <v>6575</v>
+        <v>5619</v>
       </c>
     </row>
     <row r="2760" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2760" s="1" t="s">
-        <v>5618</v>
+        <v>5620</v>
       </c>
       <c r="B2760" t="s">
         <v>5563</v>
@@ -82545,12 +82565,12 @@
         <v>1790</v>
       </c>
       <c r="P2760" t="s">
-        <v>5619</v>
+        <v>6576</v>
       </c>
     </row>
     <row r="2761" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2761" s="1" t="s">
-        <v>5620</v>
+        <v>5621</v>
       </c>
       <c r="B2761" t="s">
         <v>5563</v>
@@ -82565,12 +82585,12 @@
         <v>1790</v>
       </c>
       <c r="P2761" t="s">
-        <v>6576</v>
+        <v>5622</v>
       </c>
     </row>
     <row r="2762" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2762" s="1" t="s">
-        <v>5621</v>
+        <v>5623</v>
       </c>
       <c r="B2762" t="s">
         <v>5563</v>
@@ -82585,12 +82605,12 @@
         <v>1790</v>
       </c>
       <c r="P2762" t="s">
-        <v>5622</v>
+        <v>5624</v>
       </c>
     </row>
     <row r="2763" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2763" s="1" t="s">
-        <v>5623</v>
+        <v>5625</v>
       </c>
       <c r="B2763" t="s">
         <v>5563</v>
@@ -82605,12 +82625,12 @@
         <v>1790</v>
       </c>
       <c r="P2763" t="s">
-        <v>5624</v>
+        <v>6577</v>
       </c>
     </row>
     <row r="2764" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2764" s="1" t="s">
-        <v>5625</v>
+        <v>5626</v>
       </c>
       <c r="B2764" t="s">
         <v>5563</v>
@@ -82625,12 +82645,12 @@
         <v>1790</v>
       </c>
       <c r="P2764" t="s">
-        <v>6577</v>
+        <v>6578</v>
       </c>
     </row>
     <row r="2765" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2765" s="1" t="s">
-        <v>5626</v>
+        <v>5627</v>
       </c>
       <c r="B2765" t="s">
         <v>5563</v>
@@ -82645,12 +82665,12 @@
         <v>1790</v>
       </c>
       <c r="P2765" t="s">
-        <v>6578</v>
+        <v>5628</v>
       </c>
     </row>
     <row r="2766" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2766" s="1" t="s">
-        <v>5627</v>
+        <v>5629</v>
       </c>
       <c r="B2766" t="s">
         <v>5563</v>
@@ -82665,12 +82685,12 @@
         <v>1790</v>
       </c>
       <c r="P2766" t="s">
-        <v>5628</v>
+        <v>6579</v>
       </c>
     </row>
     <row r="2767" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2767" s="1" t="s">
-        <v>5629</v>
+        <v>5630</v>
       </c>
       <c r="B2767" t="s">
         <v>5563</v>
@@ -82685,12 +82705,12 @@
         <v>1790</v>
       </c>
       <c r="P2767" t="s">
-        <v>6579</v>
+        <v>6580</v>
       </c>
     </row>
     <row r="2768" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2768" s="1" t="s">
-        <v>5630</v>
+        <v>5631</v>
       </c>
       <c r="B2768" t="s">
         <v>5563</v>
@@ -82705,12 +82725,12 @@
         <v>1790</v>
       </c>
       <c r="P2768" t="s">
-        <v>6580</v>
+        <v>6581</v>
       </c>
     </row>
     <row r="2769" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2769" s="1" t="s">
-        <v>5631</v>
+        <v>5632</v>
       </c>
       <c r="B2769" t="s">
         <v>5563</v>
@@ -82725,12 +82745,12 @@
         <v>1790</v>
       </c>
       <c r="P2769" t="s">
-        <v>6581</v>
+        <v>6582</v>
       </c>
     </row>
     <row r="2770" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2770" s="1" t="s">
-        <v>5632</v>
+        <v>5633</v>
       </c>
       <c r="B2770" t="s">
         <v>5563</v>
@@ -82745,12 +82765,12 @@
         <v>1790</v>
       </c>
       <c r="P2770" t="s">
-        <v>6582</v>
+        <v>6583</v>
       </c>
     </row>
     <row r="2771" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2771" s="1" t="s">
-        <v>5633</v>
+        <v>5634</v>
       </c>
       <c r="B2771" t="s">
         <v>5563</v>
@@ -82765,12 +82785,12 @@
         <v>1790</v>
       </c>
       <c r="P2771" t="s">
-        <v>6583</v>
+        <v>6584</v>
       </c>
     </row>
     <row r="2772" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2772" s="1" t="s">
-        <v>5634</v>
+        <v>5635</v>
       </c>
       <c r="B2772" t="s">
         <v>5563</v>
@@ -82785,12 +82805,12 @@
         <v>1790</v>
       </c>
       <c r="P2772" t="s">
-        <v>6584</v>
+        <v>6585</v>
       </c>
     </row>
     <row r="2773" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2773" s="1" t="s">
-        <v>5635</v>
+        <v>5636</v>
       </c>
       <c r="B2773" t="s">
         <v>5563</v>
@@ -82805,12 +82825,12 @@
         <v>1790</v>
       </c>
       <c r="P2773" t="s">
-        <v>6585</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="2774" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2774" s="1" t="s">
-        <v>5636</v>
+        <v>5638</v>
       </c>
       <c r="B2774" t="s">
         <v>5563</v>
@@ -82825,12 +82845,12 @@
         <v>1790</v>
       </c>
       <c r="P2774" t="s">
-        <v>5637</v>
+        <v>5639</v>
       </c>
     </row>
     <row r="2775" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2775" s="1" t="s">
-        <v>5638</v>
+        <v>5640</v>
       </c>
       <c r="B2775" t="s">
         <v>5563</v>
@@ -82845,12 +82865,12 @@
         <v>1790</v>
       </c>
       <c r="P2775" t="s">
-        <v>5639</v>
+        <v>5641</v>
       </c>
     </row>
     <row r="2776" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2776" s="1" t="s">
-        <v>5640</v>
+        <v>5642</v>
       </c>
       <c r="B2776" t="s">
         <v>5563</v>
@@ -82865,12 +82885,12 @@
         <v>1790</v>
       </c>
       <c r="P2776" t="s">
-        <v>5641</v>
+        <v>6586</v>
       </c>
     </row>
     <row r="2777" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2777" s="1" t="s">
-        <v>5642</v>
+        <v>5643</v>
       </c>
       <c r="B2777" t="s">
         <v>5563</v>
@@ -82885,12 +82905,12 @@
         <v>1790</v>
       </c>
       <c r="P2777" t="s">
-        <v>6586</v>
+        <v>5644</v>
       </c>
     </row>
     <row r="2778" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2778" s="1" t="s">
-        <v>5643</v>
+        <v>5645</v>
       </c>
       <c r="B2778" t="s">
         <v>5563</v>
@@ -82905,12 +82925,12 @@
         <v>1790</v>
       </c>
       <c r="P2778" t="s">
-        <v>5644</v>
+        <v>5646</v>
       </c>
     </row>
     <row r="2779" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2779" s="1" t="s">
-        <v>5645</v>
+        <v>5647</v>
       </c>
       <c r="B2779" t="s">
         <v>5563</v>
@@ -82925,12 +82945,12 @@
         <v>1790</v>
       </c>
       <c r="P2779" t="s">
-        <v>5646</v>
+        <v>6587</v>
       </c>
     </row>
     <row r="2780" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2780" s="1" t="s">
-        <v>5647</v>
+        <v>5648</v>
       </c>
       <c r="B2780" t="s">
         <v>5563</v>
@@ -82945,12 +82965,12 @@
         <v>1790</v>
       </c>
       <c r="P2780" t="s">
-        <v>6587</v>
+        <v>5649</v>
       </c>
     </row>
     <row r="2781" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2781" s="1" t="s">
-        <v>5648</v>
+        <v>5650</v>
       </c>
       <c r="B2781" t="s">
         <v>5563</v>
@@ -82965,12 +82985,12 @@
         <v>1790</v>
       </c>
       <c r="P2781" t="s">
-        <v>5649</v>
+        <v>6588</v>
       </c>
     </row>
     <row r="2782" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2782" s="1" t="s">
-        <v>5650</v>
+        <v>5651</v>
       </c>
       <c r="B2782" t="s">
         <v>5563</v>
@@ -82985,12 +83005,12 @@
         <v>1790</v>
       </c>
       <c r="P2782" t="s">
-        <v>6588</v>
+        <v>6589</v>
       </c>
     </row>
     <row r="2783" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2783" s="1" t="s">
-        <v>5651</v>
+        <v>5652</v>
       </c>
       <c r="B2783" t="s">
         <v>5563</v>
@@ -83005,12 +83025,12 @@
         <v>1790</v>
       </c>
       <c r="P2783" t="s">
-        <v>6589</v>
+        <v>6590</v>
       </c>
     </row>
     <row r="2784" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2784" s="1" t="s">
-        <v>5652</v>
+        <v>5653</v>
       </c>
       <c r="B2784" t="s">
         <v>5563</v>
@@ -83025,12 +83045,12 @@
         <v>1790</v>
       </c>
       <c r="P2784" t="s">
-        <v>6590</v>
+        <v>6591</v>
       </c>
     </row>
     <row r="2785" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2785" s="1" t="s">
-        <v>5653</v>
+        <v>5654</v>
       </c>
       <c r="B2785" t="s">
         <v>5563</v>
@@ -83045,12 +83065,12 @@
         <v>1790</v>
       </c>
       <c r="P2785" t="s">
-        <v>6591</v>
+        <v>6592</v>
       </c>
     </row>
     <row r="2786" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2786" s="1" t="s">
-        <v>5654</v>
+        <v>5655</v>
       </c>
       <c r="B2786" t="s">
         <v>5563</v>
@@ -83065,12 +83085,12 @@
         <v>1790</v>
       </c>
       <c r="P2786" t="s">
-        <v>6592</v>
+        <v>6593</v>
       </c>
     </row>
     <row r="2787" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2787" s="1" t="s">
-        <v>5655</v>
+        <v>5656</v>
       </c>
       <c r="B2787" t="s">
         <v>5563</v>
@@ -83085,12 +83105,12 @@
         <v>1790</v>
       </c>
       <c r="P2787" t="s">
-        <v>6593</v>
+        <v>5657</v>
       </c>
     </row>
     <row r="2788" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2788" s="1" t="s">
-        <v>5656</v>
+        <v>5658</v>
       </c>
       <c r="B2788" t="s">
         <v>5563</v>
@@ -83105,12 +83125,12 @@
         <v>1790</v>
       </c>
       <c r="P2788" t="s">
-        <v>5657</v>
+        <v>6594</v>
       </c>
     </row>
     <row r="2789" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2789" s="1" t="s">
-        <v>5658</v>
+        <v>5659</v>
       </c>
       <c r="B2789" t="s">
         <v>5563</v>
@@ -83125,12 +83145,12 @@
         <v>1790</v>
       </c>
       <c r="P2789" t="s">
-        <v>6594</v>
+        <v>6595</v>
       </c>
     </row>
     <row r="2790" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2790" s="1" t="s">
-        <v>5659</v>
+        <v>5660</v>
       </c>
       <c r="B2790" t="s">
         <v>5563</v>
@@ -83145,12 +83165,12 @@
         <v>1790</v>
       </c>
       <c r="P2790" t="s">
-        <v>6595</v>
+        <v>5661</v>
       </c>
     </row>
     <row r="2791" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2791" s="1" t="s">
-        <v>5660</v>
+        <v>5662</v>
       </c>
       <c r="B2791" t="s">
         <v>5563</v>
@@ -83165,12 +83185,12 @@
         <v>1790</v>
       </c>
       <c r="P2791" t="s">
-        <v>5661</v>
+        <v>5663</v>
       </c>
     </row>
     <row r="2792" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2792" s="1" t="s">
-        <v>5662</v>
+        <v>5664</v>
       </c>
       <c r="B2792" t="s">
         <v>5563</v>
@@ -83185,12 +83205,12 @@
         <v>1790</v>
       </c>
       <c r="P2792" t="s">
-        <v>5663</v>
+        <v>6596</v>
       </c>
     </row>
     <row r="2793" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2793" s="1" t="s">
-        <v>5664</v>
+        <v>5665</v>
       </c>
       <c r="B2793" t="s">
         <v>5563</v>
@@ -83205,12 +83225,12 @@
         <v>1790</v>
       </c>
       <c r="P2793" t="s">
-        <v>6596</v>
+        <v>5666</v>
       </c>
     </row>
     <row r="2794" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2794" s="1" t="s">
-        <v>5665</v>
+        <v>5667</v>
       </c>
       <c r="B2794" t="s">
         <v>5563</v>
@@ -83225,12 +83245,12 @@
         <v>1790</v>
       </c>
       <c r="P2794" t="s">
-        <v>5666</v>
+        <v>6597</v>
       </c>
     </row>
     <row r="2795" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2795" s="1" t="s">
-        <v>5667</v>
+        <v>5668</v>
       </c>
       <c r="B2795" t="s">
         <v>5563</v>
@@ -83245,12 +83265,12 @@
         <v>1790</v>
       </c>
       <c r="P2795" t="s">
-        <v>6597</v>
+        <v>6598</v>
       </c>
     </row>
     <row r="2796" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2796" s="1" t="s">
-        <v>5668</v>
+        <v>5669</v>
       </c>
       <c r="B2796" t="s">
         <v>5563</v>
@@ -83265,12 +83285,12 @@
         <v>1790</v>
       </c>
       <c r="P2796" t="s">
-        <v>6598</v>
+        <v>6599</v>
       </c>
     </row>
     <row r="2797" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2797" s="1" t="s">
-        <v>5669</v>
+        <v>5670</v>
       </c>
       <c r="B2797" t="s">
         <v>5563</v>
@@ -83285,12 +83305,12 @@
         <v>1790</v>
       </c>
       <c r="P2797" t="s">
-        <v>6599</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="2798" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2798" s="1" t="s">
-        <v>5670</v>
+        <v>5671</v>
       </c>
       <c r="B2798" t="s">
         <v>5563</v>
@@ -83305,12 +83325,12 @@
         <v>1790</v>
       </c>
       <c r="P2798" t="s">
-        <v>6600</v>
+        <v>6601</v>
       </c>
     </row>
     <row r="2799" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2799" s="1" t="s">
-        <v>5671</v>
+        <v>5672</v>
       </c>
       <c r="B2799" t="s">
         <v>5563</v>
@@ -83325,12 +83345,12 @@
         <v>1790</v>
       </c>
       <c r="P2799" t="s">
-        <v>6601</v>
+        <v>5673</v>
       </c>
     </row>
     <row r="2800" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2800" s="1" t="s">
-        <v>5672</v>
+        <v>5674</v>
       </c>
       <c r="B2800" t="s">
         <v>5563</v>
@@ -83345,12 +83365,12 @@
         <v>1790</v>
       </c>
       <c r="P2800" t="s">
-        <v>5673</v>
+        <v>6602</v>
       </c>
     </row>
     <row r="2801" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2801" s="1" t="s">
-        <v>5674</v>
+        <v>5675</v>
       </c>
       <c r="B2801" t="s">
         <v>5563</v>
@@ -83365,12 +83385,12 @@
         <v>1790</v>
       </c>
       <c r="P2801" t="s">
-        <v>6602</v>
+        <v>5676</v>
       </c>
     </row>
     <row r="2802" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2802" s="1" t="s">
-        <v>5675</v>
+        <v>5677</v>
       </c>
       <c r="B2802" t="s">
         <v>5563</v>
@@ -83385,12 +83405,12 @@
         <v>1790</v>
       </c>
       <c r="P2802" t="s">
-        <v>5676</v>
+        <v>6603</v>
       </c>
     </row>
     <row r="2803" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2803" s="1" t="s">
-        <v>5677</v>
+        <v>5678</v>
       </c>
       <c r="B2803" t="s">
         <v>5563</v>
@@ -83405,12 +83425,12 @@
         <v>1790</v>
       </c>
       <c r="P2803" t="s">
-        <v>6603</v>
+        <v>5679</v>
       </c>
     </row>
     <row r="2804" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2804" s="1" t="s">
-        <v>5678</v>
+        <v>5680</v>
       </c>
       <c r="B2804" t="s">
         <v>5563</v>
@@ -83425,12 +83445,12 @@
         <v>1790</v>
       </c>
       <c r="P2804" t="s">
-        <v>5679</v>
+        <v>5681</v>
       </c>
     </row>
     <row r="2805" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2805" s="1" t="s">
-        <v>5680</v>
+        <v>5682</v>
       </c>
       <c r="B2805" t="s">
         <v>5563</v>
@@ -83445,12 +83465,12 @@
         <v>1790</v>
       </c>
       <c r="P2805" t="s">
-        <v>5681</v>
+        <v>6604</v>
       </c>
     </row>
     <row r="2806" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2806" s="1" t="s">
-        <v>5682</v>
+        <v>5683</v>
       </c>
       <c r="B2806" t="s">
         <v>5563</v>
@@ -83465,12 +83485,12 @@
         <v>1790</v>
       </c>
       <c r="P2806" t="s">
-        <v>6604</v>
+        <v>6605</v>
       </c>
     </row>
     <row r="2807" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2807" s="1" t="s">
-        <v>5683</v>
+        <v>5684</v>
       </c>
       <c r="B2807" t="s">
         <v>5563</v>
@@ -83485,12 +83505,12 @@
         <v>1790</v>
       </c>
       <c r="P2807" t="s">
-        <v>6605</v>
+        <v>5685</v>
       </c>
     </row>
     <row r="2808" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2808" s="1" t="s">
-        <v>5684</v>
+        <v>5686</v>
       </c>
       <c r="B2808" t="s">
         <v>5563</v>
@@ -83505,12 +83525,12 @@
         <v>1790</v>
       </c>
       <c r="P2808" t="s">
-        <v>5685</v>
+        <v>5687</v>
       </c>
     </row>
     <row r="2809" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2809" s="1" t="s">
-        <v>5686</v>
+        <v>5688</v>
       </c>
       <c r="B2809" t="s">
         <v>5563</v>
@@ -83525,12 +83545,12 @@
         <v>1790</v>
       </c>
       <c r="P2809" t="s">
-        <v>5687</v>
+        <v>6606</v>
       </c>
     </row>
     <row r="2810" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2810" s="1" t="s">
-        <v>5688</v>
+        <v>5689</v>
       </c>
       <c r="B2810" t="s">
         <v>5563</v>
@@ -83545,12 +83565,12 @@
         <v>1790</v>
       </c>
       <c r="P2810" t="s">
-        <v>6606</v>
+        <v>5690</v>
       </c>
     </row>
     <row r="2811" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2811" s="1" t="s">
-        <v>5689</v>
+        <v>5691</v>
       </c>
       <c r="B2811" t="s">
         <v>5563</v>
@@ -83565,12 +83585,12 @@
         <v>1790</v>
       </c>
       <c r="P2811" t="s">
-        <v>5690</v>
+        <v>6607</v>
       </c>
     </row>
     <row r="2812" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2812" s="1" t="s">
-        <v>5691</v>
+        <v>5692</v>
       </c>
       <c r="B2812" t="s">
         <v>5563</v>
@@ -83585,12 +83605,12 @@
         <v>1790</v>
       </c>
       <c r="P2812" t="s">
-        <v>6607</v>
+        <v>6608</v>
       </c>
     </row>
     <row r="2813" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2813" s="1" t="s">
-        <v>5692</v>
+        <v>5693</v>
       </c>
       <c r="B2813" t="s">
         <v>5563</v>
@@ -83605,12 +83625,12 @@
         <v>1790</v>
       </c>
       <c r="P2813" t="s">
-        <v>6608</v>
+        <v>6609</v>
       </c>
     </row>
     <row r="2814" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2814" s="1" t="s">
-        <v>5693</v>
+        <v>5694</v>
       </c>
       <c r="B2814" t="s">
         <v>5563</v>
@@ -83625,12 +83645,12 @@
         <v>1790</v>
       </c>
       <c r="P2814" t="s">
-        <v>6609</v>
+        <v>6610</v>
       </c>
     </row>
     <row r="2815" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2815" s="1" t="s">
-        <v>5694</v>
+        <v>5695</v>
       </c>
       <c r="B2815" t="s">
         <v>5563</v>
@@ -83645,12 +83665,12 @@
         <v>1790</v>
       </c>
       <c r="P2815" t="s">
-        <v>6610</v>
+        <v>6611</v>
       </c>
     </row>
     <row r="2816" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2816" s="1" t="s">
-        <v>5695</v>
+        <v>5696</v>
       </c>
       <c r="B2816" t="s">
         <v>5563</v>
@@ -83665,12 +83685,12 @@
         <v>1790</v>
       </c>
       <c r="P2816" t="s">
-        <v>6611</v>
+        <v>6612</v>
       </c>
     </row>
     <row r="2817" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2817" s="1" t="s">
-        <v>5696</v>
+        <v>5697</v>
       </c>
       <c r="B2817" t="s">
         <v>5563</v>
@@ -83685,12 +83705,12 @@
         <v>1790</v>
       </c>
       <c r="P2817" t="s">
-        <v>6612</v>
+        <v>5698</v>
       </c>
     </row>
     <row r="2818" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2818" s="1" t="s">
-        <v>5697</v>
+        <v>5699</v>
       </c>
       <c r="B2818" t="s">
         <v>5563</v>
@@ -83705,12 +83725,12 @@
         <v>1790</v>
       </c>
       <c r="P2818" t="s">
-        <v>5698</v>
+        <v>6613</v>
       </c>
     </row>
     <row r="2819" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2819" s="1" t="s">
-        <v>5699</v>
+        <v>5700</v>
       </c>
       <c r="B2819" t="s">
         <v>5563</v>
@@ -83725,12 +83745,12 @@
         <v>1790</v>
       </c>
       <c r="P2819" t="s">
-        <v>6613</v>
+        <v>6614</v>
       </c>
     </row>
     <row r="2820" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2820" s="1" t="s">
-        <v>5700</v>
+        <v>5701</v>
       </c>
       <c r="B2820" t="s">
         <v>5563</v>
@@ -83745,12 +83765,12 @@
         <v>1790</v>
       </c>
       <c r="P2820" t="s">
-        <v>6614</v>
+        <v>5702</v>
       </c>
     </row>
     <row r="2821" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2821" s="1" t="s">
-        <v>5701</v>
+        <v>5703</v>
       </c>
       <c r="B2821" t="s">
         <v>5563</v>
@@ -83765,12 +83785,12 @@
         <v>1790</v>
       </c>
       <c r="P2821" t="s">
-        <v>5702</v>
+        <v>6615</v>
       </c>
     </row>
     <row r="2822" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2822" s="1" t="s">
-        <v>5703</v>
+        <v>5704</v>
       </c>
       <c r="B2822" t="s">
         <v>5563</v>
@@ -83785,12 +83805,12 @@
         <v>1790</v>
       </c>
       <c r="P2822" t="s">
-        <v>6615</v>
+        <v>5705</v>
       </c>
     </row>
     <row r="2823" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2823" s="1" t="s">
-        <v>5704</v>
+        <v>5706</v>
       </c>
       <c r="B2823" t="s">
         <v>5563</v>
@@ -83805,12 +83825,12 @@
         <v>1790</v>
       </c>
       <c r="P2823" t="s">
-        <v>5705</v>
+        <v>5707</v>
       </c>
     </row>
     <row r="2824" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2824" s="1" t="s">
-        <v>5706</v>
+        <v>5708</v>
       </c>
       <c r="B2824" t="s">
         <v>5563</v>
@@ -83825,12 +83845,12 @@
         <v>1790</v>
       </c>
       <c r="P2824" t="s">
-        <v>5707</v>
+        <v>6616</v>
       </c>
     </row>
     <row r="2825" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2825" s="1" t="s">
-        <v>5708</v>
+        <v>5709</v>
       </c>
       <c r="B2825" t="s">
         <v>5563</v>
@@ -83845,12 +83865,12 @@
         <v>1790</v>
       </c>
       <c r="P2825" t="s">
-        <v>6616</v>
+        <v>5710</v>
       </c>
     </row>
     <row r="2826" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2826" s="1" t="s">
-        <v>5709</v>
+        <v>5711</v>
       </c>
       <c r="B2826" t="s">
         <v>5563</v>
@@ -83865,12 +83885,12 @@
         <v>1790</v>
       </c>
       <c r="P2826" t="s">
-        <v>5710</v>
+        <v>6617</v>
       </c>
     </row>
     <row r="2827" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2827" s="1" t="s">
-        <v>5711</v>
+        <v>5712</v>
       </c>
       <c r="B2827" t="s">
         <v>5563</v>
@@ -83885,12 +83905,12 @@
         <v>1790</v>
       </c>
       <c r="P2827" t="s">
-        <v>6617</v>
+        <v>6618</v>
       </c>
     </row>
     <row r="2828" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2828" s="1" t="s">
-        <v>5712</v>
+        <v>5713</v>
       </c>
       <c r="B2828" t="s">
         <v>5563</v>
@@ -83905,12 +83925,12 @@
         <v>1790</v>
       </c>
       <c r="P2828" t="s">
-        <v>6618</v>
+        <v>6619</v>
       </c>
     </row>
     <row r="2829" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2829" s="1" t="s">
-        <v>5713</v>
+        <v>5714</v>
       </c>
       <c r="B2829" t="s">
         <v>5563</v>
@@ -83925,12 +83945,12 @@
         <v>1790</v>
       </c>
       <c r="P2829" t="s">
-        <v>6619</v>
+        <v>6620</v>
       </c>
     </row>
     <row r="2830" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2830" s="1" t="s">
-        <v>5714</v>
+        <v>5715</v>
       </c>
       <c r="B2830" t="s">
         <v>5563</v>
@@ -83945,12 +83965,12 @@
         <v>1790</v>
       </c>
       <c r="P2830" t="s">
-        <v>6620</v>
+        <v>6621</v>
       </c>
     </row>
     <row r="2831" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2831" s="1" t="s">
-        <v>5715</v>
+        <v>5716</v>
       </c>
       <c r="B2831" t="s">
         <v>5563</v>
@@ -83965,12 +83985,12 @@
         <v>1790</v>
       </c>
       <c r="P2831" t="s">
-        <v>6621</v>
+        <v>5717</v>
       </c>
     </row>
     <row r="2832" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2832" s="1" t="s">
-        <v>5716</v>
+        <v>5718</v>
       </c>
       <c r="B2832" t="s">
         <v>5563</v>
@@ -83985,12 +84005,12 @@
         <v>1790</v>
       </c>
       <c r="P2832" t="s">
-        <v>5717</v>
+        <v>6622</v>
       </c>
     </row>
     <row r="2833" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2833" s="1" t="s">
-        <v>5718</v>
+        <v>5719</v>
       </c>
       <c r="B2833" t="s">
         <v>5563</v>
@@ -84005,12 +84025,12 @@
         <v>1790</v>
       </c>
       <c r="P2833" t="s">
-        <v>6622</v>
+        <v>6623</v>
       </c>
     </row>
     <row r="2834" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2834" s="1" t="s">
-        <v>5719</v>
+        <v>5720</v>
       </c>
       <c r="B2834" t="s">
         <v>5563</v>
@@ -84025,12 +84045,12 @@
         <v>1790</v>
       </c>
       <c r="P2834" t="s">
-        <v>6623</v>
+        <v>5721</v>
       </c>
     </row>
     <row r="2835" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2835" s="1" t="s">
-        <v>5720</v>
+        <v>5722</v>
       </c>
       <c r="B2835" t="s">
         <v>5563</v>
@@ -84045,12 +84065,12 @@
         <v>1790</v>
       </c>
       <c r="P2835" t="s">
-        <v>5721</v>
+        <v>5723</v>
       </c>
     </row>
     <row r="2836" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2836" s="1" t="s">
-        <v>5722</v>
+        <v>5724</v>
       </c>
       <c r="B2836" t="s">
         <v>5563</v>
@@ -84065,12 +84085,12 @@
         <v>1790</v>
       </c>
       <c r="P2836" t="s">
-        <v>5723</v>
+        <v>5725</v>
       </c>
     </row>
     <row r="2837" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2837" s="1" t="s">
-        <v>5724</v>
+        <v>5726</v>
       </c>
       <c r="B2837" t="s">
         <v>5563</v>
@@ -84085,12 +84105,12 @@
         <v>1790</v>
       </c>
       <c r="P2837" t="s">
-        <v>5725</v>
+        <v>5727</v>
       </c>
     </row>
     <row r="2838" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2838" s="1" t="s">
-        <v>5726</v>
+        <v>5728</v>
       </c>
       <c r="B2838" t="s">
         <v>5563</v>
@@ -84105,12 +84125,12 @@
         <v>1790</v>
       </c>
       <c r="P2838" t="s">
-        <v>5727</v>
+        <v>6624</v>
       </c>
     </row>
     <row r="2839" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2839" s="1" t="s">
-        <v>5728</v>
+        <v>5729</v>
       </c>
       <c r="B2839" t="s">
         <v>5563</v>
@@ -84125,12 +84145,12 @@
         <v>1790</v>
       </c>
       <c r="P2839" t="s">
-        <v>6624</v>
+        <v>5730</v>
       </c>
     </row>
     <row r="2840" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2840" s="1" t="s">
-        <v>5729</v>
+        <v>5731</v>
       </c>
       <c r="B2840" t="s">
         <v>5563</v>
@@ -84145,12 +84165,12 @@
         <v>1790</v>
       </c>
       <c r="P2840" t="s">
-        <v>5730</v>
+        <v>5732</v>
       </c>
     </row>
     <row r="2841" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2841" s="1" t="s">
-        <v>5731</v>
+        <v>5733</v>
       </c>
       <c r="B2841" t="s">
         <v>5563</v>
@@ -84165,12 +84185,12 @@
         <v>1790</v>
       </c>
       <c r="P2841" t="s">
-        <v>5732</v>
+        <v>6625</v>
       </c>
     </row>
     <row r="2842" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2842" s="1" t="s">
-        <v>5733</v>
+        <v>5734</v>
       </c>
       <c r="B2842" t="s">
         <v>5563</v>
@@ -84185,12 +84205,12 @@
         <v>1790</v>
       </c>
       <c r="P2842" t="s">
-        <v>6625</v>
+        <v>5735</v>
       </c>
     </row>
     <row r="2843" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2843" s="1" t="s">
-        <v>5734</v>
+        <v>5736</v>
       </c>
       <c r="B2843" t="s">
         <v>5563</v>
@@ -84205,12 +84225,12 @@
         <v>1790</v>
       </c>
       <c r="P2843" t="s">
-        <v>5735</v>
+        <v>6626</v>
       </c>
     </row>
     <row r="2844" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2844" s="1" t="s">
-        <v>5736</v>
+        <v>5737</v>
       </c>
       <c r="B2844" t="s">
         <v>5563</v>
@@ -84225,12 +84245,12 @@
         <v>1790</v>
       </c>
       <c r="P2844" t="s">
-        <v>6626</v>
+        <v>5738</v>
       </c>
     </row>
     <row r="2845" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2845" s="1" t="s">
-        <v>5737</v>
+        <v>5739</v>
       </c>
       <c r="B2845" t="s">
         <v>5563</v>
@@ -84245,12 +84265,12 @@
         <v>1790</v>
       </c>
       <c r="P2845" t="s">
-        <v>5738</v>
+        <v>5740</v>
       </c>
     </row>
     <row r="2846" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2846" s="1" t="s">
-        <v>5739</v>
+        <v>5741</v>
       </c>
       <c r="B2846" t="s">
         <v>5563</v>
@@ -84265,12 +84285,12 @@
         <v>1790</v>
       </c>
       <c r="P2846" t="s">
-        <v>5740</v>
+        <v>5742</v>
       </c>
     </row>
     <row r="2847" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2847" s="1" t="s">
-        <v>5741</v>
+        <v>5743</v>
       </c>
       <c r="B2847" t="s">
         <v>5563</v>
@@ -84285,12 +84305,12 @@
         <v>1790</v>
       </c>
       <c r="P2847" t="s">
-        <v>5742</v>
+        <v>5744</v>
       </c>
     </row>
     <row r="2848" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2848" s="1" t="s">
-        <v>5743</v>
+        <v>5745</v>
       </c>
       <c r="B2848" t="s">
         <v>5563</v>
@@ -84305,12 +84325,12 @@
         <v>1790</v>
       </c>
       <c r="P2848" t="s">
-        <v>5744</v>
+        <v>6627</v>
       </c>
     </row>
     <row r="2849" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2849" s="1" t="s">
-        <v>5745</v>
+        <v>5746</v>
       </c>
       <c r="B2849" t="s">
         <v>5563</v>
@@ -84325,12 +84345,12 @@
         <v>1790</v>
       </c>
       <c r="P2849" t="s">
-        <v>6627</v>
+        <v>6628</v>
       </c>
     </row>
     <row r="2850" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2850" s="1" t="s">
-        <v>5746</v>
+        <v>5747</v>
       </c>
       <c r="B2850" t="s">
         <v>5563</v>
@@ -84345,12 +84365,12 @@
         <v>1790</v>
       </c>
       <c r="P2850" t="s">
-        <v>6628</v>
+        <v>6629</v>
       </c>
     </row>
     <row r="2851" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2851" s="1" t="s">
-        <v>5747</v>
+        <v>5748</v>
       </c>
       <c r="B2851" t="s">
         <v>5563</v>
@@ -84365,12 +84385,12 @@
         <v>1790</v>
       </c>
       <c r="P2851" t="s">
-        <v>6629</v>
+        <v>6630</v>
       </c>
     </row>
     <row r="2852" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2852" s="1" t="s">
-        <v>5748</v>
+        <v>5749</v>
       </c>
       <c r="B2852" t="s">
         <v>5563</v>
@@ -84385,12 +84405,12 @@
         <v>1790</v>
       </c>
       <c r="P2852" t="s">
-        <v>6630</v>
+        <v>6631</v>
       </c>
     </row>
     <row r="2853" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2853" s="1" t="s">
-        <v>5749</v>
+        <v>5750</v>
       </c>
       <c r="B2853" t="s">
         <v>5563</v>
@@ -84405,12 +84425,12 @@
         <v>1790</v>
       </c>
       <c r="P2853" t="s">
-        <v>6631</v>
+        <v>5751</v>
       </c>
     </row>
     <row r="2854" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2854" s="1" t="s">
-        <v>5750</v>
+        <v>5752</v>
       </c>
       <c r="B2854" t="s">
         <v>5563</v>
@@ -84425,12 +84445,12 @@
         <v>1790</v>
       </c>
       <c r="P2854" t="s">
-        <v>5751</v>
+        <v>6632</v>
       </c>
     </row>
     <row r="2855" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2855" s="1" t="s">
-        <v>5752</v>
+        <v>5753</v>
       </c>
       <c r="B2855" t="s">
         <v>5563</v>
@@ -84445,12 +84465,12 @@
         <v>1790</v>
       </c>
       <c r="P2855" t="s">
-        <v>6632</v>
+        <v>5754</v>
       </c>
     </row>
     <row r="2856" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2856" s="1" t="s">
-        <v>5753</v>
+        <v>5755</v>
       </c>
       <c r="B2856" t="s">
         <v>5563</v>
@@ -84465,12 +84485,12 @@
         <v>1790</v>
       </c>
       <c r="P2856" t="s">
-        <v>5754</v>
+        <v>6633</v>
       </c>
     </row>
     <row r="2857" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2857" s="1" t="s">
-        <v>5755</v>
+        <v>5756</v>
       </c>
       <c r="B2857" t="s">
         <v>5563</v>
@@ -84485,12 +84505,12 @@
         <v>1790</v>
       </c>
       <c r="P2857" t="s">
-        <v>6633</v>
+        <v>5757</v>
       </c>
     </row>
     <row r="2858" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2858" s="1" t="s">
-        <v>5756</v>
+        <v>5758</v>
       </c>
       <c r="B2858" t="s">
         <v>5563</v>
@@ -84505,12 +84525,12 @@
         <v>1790</v>
       </c>
       <c r="P2858" t="s">
-        <v>5757</v>
+        <v>6634</v>
       </c>
     </row>
     <row r="2859" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2859" s="1" t="s">
-        <v>5758</v>
+        <v>5759</v>
       </c>
       <c r="B2859" t="s">
         <v>5563</v>
@@ -84525,12 +84545,12 @@
         <v>1790</v>
       </c>
       <c r="P2859" t="s">
-        <v>6634</v>
+        <v>6635</v>
       </c>
     </row>
     <row r="2860" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2860" s="1" t="s">
-        <v>5759</v>
+        <v>5760</v>
       </c>
       <c r="B2860" t="s">
         <v>5563</v>
@@ -84545,12 +84565,12 @@
         <v>1790</v>
       </c>
       <c r="P2860" t="s">
-        <v>6635</v>
+        <v>6636</v>
       </c>
     </row>
     <row r="2861" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2861" s="1" t="s">
-        <v>5760</v>
+        <v>5761</v>
       </c>
       <c r="B2861" t="s">
         <v>5563</v>
@@ -84565,26 +84585,6 @@
         <v>1790</v>
       </c>
       <c r="P2861" t="s">
-        <v>6636</v>
-      </c>
-    </row>
-    <row r="2862" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2862" s="1" t="s">
-        <v>5761</v>
-      </c>
-      <c r="B2862" t="s">
-        <v>5563</v>
-      </c>
-      <c r="C2862">
-        <v>68000</v>
-      </c>
-      <c r="D2862" t="s">
-        <v>168</v>
-      </c>
-      <c r="K2862" t="s">
-        <v>1790</v>
-      </c>
-      <c r="P2862" t="s">
         <v>6637</v>
       </c>
     </row>

</xml_diff>